<commit_message>
Actualizacion del Estudio Finaciero
</commit_message>
<xml_diff>
--- a/Estudio_financiero.xlsx
+++ b/Estudio_financiero.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" tabRatio="493" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Demanda Dinamica" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="322">
   <si>
     <t>INFORMACIÓN PARA TENER EN CUENTA:</t>
   </si>
@@ -703,22 +703,313 @@
   </si>
   <si>
     <t>TOTAL GASTOS ADICIONALES</t>
+  </si>
+  <si>
+    <t>PRESUPUESTO DE GASTOS DE ADMINITRACION</t>
+  </si>
+  <si>
+    <t>Personal Adminsitrativo</t>
+  </si>
+  <si>
+    <t>Gastos transporte</t>
+  </si>
+  <si>
+    <t>Gastos Papeleria</t>
+  </si>
+  <si>
+    <t>Gastos de aseo y mantenimiento de Instalaciones</t>
+  </si>
+  <si>
+    <t>Depreciacion de Muebles y enseres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amortización de Intangibles </t>
+  </si>
+  <si>
+    <t>Amortización gastos de arranque</t>
+  </si>
+  <si>
+    <t>Registro Mercantil (1er año anticip. Inves. Intang)</t>
+  </si>
+  <si>
+    <t>Bomberos (1er año anticip. Inves. Intang))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mensual </t>
+  </si>
+  <si>
+    <t>Total Gastos Adminsitracion</t>
+  </si>
+  <si>
+    <t>COSTOS DE OPERACIÓN</t>
+  </si>
+  <si>
+    <t>Costos de administración</t>
+  </si>
+  <si>
+    <t>Costos de producción</t>
+  </si>
+  <si>
+    <t>(Año 1)</t>
+  </si>
+  <si>
+    <t>(Año 2)</t>
+  </si>
+  <si>
+    <t>(Año 3)</t>
+  </si>
+  <si>
+    <t>Total costos de Operación</t>
+  </si>
+  <si>
+    <t>(Año 1 )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Año 2) </t>
+  </si>
+  <si>
+    <t>Costo Unitario</t>
+  </si>
+  <si>
+    <t>Precio de Venta</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Mayoristas</t>
+  </si>
+  <si>
+    <t>Intermediarios</t>
+  </si>
+  <si>
+    <t>Al Detal</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>% de Ventas</t>
+  </si>
+  <si>
+    <t>con</t>
+  </si>
+  <si>
+    <t>Capacidad</t>
+  </si>
+  <si>
+    <t>Rango de  Unidades de Producto/Clientes (Anual)</t>
+  </si>
+  <si>
+    <t>$ Venta/Ud o cliente Año 1</t>
+  </si>
+  <si>
+    <t>$ Venta/Ud o cliente Año 2</t>
+  </si>
+  <si>
+    <t>$ Venta/Ud o cliente Año 3</t>
+  </si>
+  <si>
+    <t>Forma de pago</t>
+  </si>
+  <si>
+    <t>PROYECCION DE PRECIOS DE VENTA POR PRODUCTO/SERVICIO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mes 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mes 2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Me 3</t>
+  </si>
+  <si>
+    <t>Mes 5</t>
+  </si>
+  <si>
+    <t>Mes 7</t>
+  </si>
+  <si>
+    <t>Mes 12</t>
+  </si>
+  <si>
+    <t>RETEIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ventas a Intermediarios </t>
+  </si>
+  <si>
+    <t>Ventas a Detal</t>
+  </si>
+  <si>
+    <t>Total Ventas Brutas ($)</t>
+  </si>
+  <si>
+    <t>Retefuente (No aplica al detal)</t>
+  </si>
+  <si>
+    <t>Ventas Netas</t>
+  </si>
+  <si>
+    <t>Valor de Ventas de contado</t>
+  </si>
+  <si>
+    <t>Recuperacion de Cartera</t>
+  </si>
+  <si>
+    <t>Ingresos Efectivos</t>
+  </si>
+  <si>
+    <t>Cuentas por Cobrar</t>
+  </si>
+  <si>
+    <t>Ventas a Plazos</t>
+  </si>
+  <si>
+    <t>PRESUPUESTO DE INGRESO</t>
+  </si>
+  <si>
+    <t>GASTOS DE VENTA</t>
+  </si>
+  <si>
+    <t>Empaque y embalaje del producto</t>
+  </si>
+  <si>
+    <t>Comisiones de Venta (% de ventas Brutas)</t>
+  </si>
+  <si>
+    <t>Gastos de publicidad (% de Ventas de Brutas)</t>
+  </si>
+  <si>
+    <t>Imp. Industria y Com ( 11*1.000 de Ventas Brutas)</t>
+  </si>
+  <si>
+    <t>Imp. Avisos y Tableros (15% Industria y Comercio)</t>
+  </si>
+  <si>
+    <t>Total Gastos de Ventas</t>
+  </si>
+  <si>
+    <t>V. Brutas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utilidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comisiones </t>
+  </si>
+  <si>
+    <t>Publicidad</t>
+  </si>
+  <si>
+    <t>Costos Fijos</t>
+  </si>
+  <si>
+    <t>Registro Mercantil (pago ant año 1)</t>
+  </si>
+  <si>
+    <t>No aplica Año 1</t>
+  </si>
+  <si>
+    <t>Bomberos ( pago anticipado año 1)</t>
+  </si>
+  <si>
+    <t>Personal de Planta</t>
+  </si>
+  <si>
+    <t>Asesoría Contable</t>
+  </si>
+  <si>
+    <t>Servicios Públicos</t>
+  </si>
+  <si>
+    <t>Seguros</t>
+  </si>
+  <si>
+    <t>Gasto Transporte</t>
+  </si>
+  <si>
+    <t>Gastos Papelería</t>
+  </si>
+  <si>
+    <t>Gastos aseo y mto Instalaciones</t>
+  </si>
+  <si>
+    <t>Amortización de Intangibles</t>
+  </si>
+  <si>
+    <t>Total Costos Fijos</t>
+  </si>
+  <si>
+    <t>Costos Variables</t>
+  </si>
+  <si>
+    <t>Aditivos/suministros</t>
+  </si>
+  <si>
+    <t>Horas Extras y Festivas</t>
+  </si>
+  <si>
+    <t>Personal Temporal</t>
+  </si>
+  <si>
+    <t>Comisiones por Ventas</t>
+  </si>
+  <si>
+    <t>Gastos de Publicidad</t>
+  </si>
+  <si>
+    <t>Industria y Comercio</t>
+  </si>
+  <si>
+    <t>Avisos y Tableros</t>
+  </si>
+  <si>
+    <t>Total Costos Variables</t>
+  </si>
+  <si>
+    <t>Costo Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CLASIFICACIÓN DE COSTOS </t>
+  </si>
+  <si>
+    <t>Impuestos Locales ( Valor 2 % Bodega)</t>
+  </si>
+  <si>
+    <t>Calculo</t>
+  </si>
+  <si>
+    <t>INDICADORES DE COSTOS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="7">
+  <numFmts count="10">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="165" formatCode="[$$-240A]\ #,##0.00"/>
     <numFmt numFmtId="166" formatCode="[$$-240A]\ #,##0"/>
     <numFmt numFmtId="167" formatCode="_-[$$-240A]\ * #,##0.00_ ;_-[$$-240A]\ * \-#,##0.00\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="168" formatCode="_-[$$-240A]\ * #,##0_ ;_-[$$-240A]\ * \-#,##0\ ;_-[$$-240A]\ * &quot;-&quot;_ ;_-@_ "/>
+    <numFmt numFmtId="179" formatCode="_-[$$-240A]\ * #,##0.0_ ;_-[$$-240A]\ * \-#,##0.0\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="180" formatCode="_-[$$-240A]\ * #,##0_ ;_-[$$-240A]\ * \-#,##0\ ;_-[$$-240A]\ * &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="182" formatCode="_-[$$-240A]\ * #,##0.0_ ;_-[$$-240A]\ * \-#,##0.0\ ;_-[$$-240A]\ * &quot;-&quot;?_ ;_-@_ "/>
+    <numFmt numFmtId="183" formatCode="_-[$$-240A]\ * #,##0_ ;_-[$$-240A]\ * \-#,##0\ ;_-[$$-240A]\ * &quot;-&quot;?_ ;_-@_ "/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -798,8 +1089,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,8 +1152,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1025,13 +1353,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="117">
+  <cellXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1149,14 +1492,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1299,6 +1648,68 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="180" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="2" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="182" fontId="2" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="14" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="2" fillId="12" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -1457,40 +1868,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>20</c:v>
+                <c:pt idx="9">
+                  <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="10">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>48</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>33</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>21</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1919,13 +2330,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>284</c:v>
+                  <c:v>214</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>357</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>524</c:v>
+                  <c:v>427</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3697,8 +4108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y59"/>
   <sheetViews>
-    <sheetView topLeftCell="S30" workbookViewId="0">
-      <selection activeCell="X42" sqref="X42"/>
+    <sheetView topLeftCell="O29" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3727,39 +4138,39 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:19">
-      <c r="A2" s="76" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
+      <c r="A2" s="78" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="112" t="s">
         <v>215</v>
       </c>
-      <c r="C4" s="77" t="s">
+      <c r="C4" s="79" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="77"/>
+      <c r="D4" s="79"/>
       <c r="I4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="4">
         <v>0.19</v>
       </c>
-      <c r="M4" s="80" t="s">
+      <c r="M4" s="82" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="81"/>
-      <c r="O4" s="79"/>
-      <c r="R4" s="71" t="s">
+      <c r="N4" s="83"/>
+      <c r="O4" s="81"/>
+      <c r="R4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="72"/>
+      <c r="S4" s="74"/>
     </row>
     <row r="5" spans="1:19">
-      <c r="A5" s="110" t="s">
+      <c r="A5" s="112" t="s">
         <v>216</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -3780,15 +4191,15 @@
       <c r="M5" s="6">
         <v>0.5</v>
       </c>
-      <c r="N5" s="78" t="s">
+      <c r="N5" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="O5" s="79"/>
-      <c r="R5" s="73"/>
-      <c r="S5" s="74"/>
+      <c r="O5" s="81"/>
+      <c r="R5" s="75"/>
+      <c r="S5" s="76"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="A6" s="110" t="s">
+      <c r="A6" s="112" t="s">
         <v>217</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -3800,10 +4211,10 @@
       <c r="M6" s="6">
         <v>0.5</v>
       </c>
-      <c r="N6" s="78" t="s">
+      <c r="N6" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="79"/>
+      <c r="O6" s="81"/>
       <c r="R6" s="7" t="s">
         <v>11</v>
       </c>
@@ -3826,24 +4237,24 @@
       </c>
     </row>
     <row r="9" spans="1:19">
-      <c r="B9" s="70" t="s">
+      <c r="B9" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="72"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="72"/>
+      <c r="O9" s="72"/>
+      <c r="P9" s="72"/>
+      <c r="Q9" s="72"/>
     </row>
     <row r="10" spans="1:19">
       <c r="B10" s="10"/>
@@ -4005,91 +4416,91 @@
       </c>
       <c r="C13" s="15">
         <f ca="1">RANDBETWEEN(C12,C11)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D13" s="15">
         <f t="shared" ref="D13:N13" ca="1" si="1">RANDBETWEEN(D12,D11)</f>
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="G13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="H13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="I13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="L13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="N13" s="15">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="O13" s="15">
         <f t="shared" ref="O13" ca="1" si="2">RANDBETWEEN(O12,O11)</f>
-        <v>284</v>
+        <v>214</v>
       </c>
       <c r="P13" s="15">
         <f t="shared" ref="P13" ca="1" si="3">RANDBETWEEN(P12,P11)</f>
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="Q13" s="15">
         <f t="shared" ref="Q13" ca="1" si="4">RANDBETWEEN(Q12,Q11)</f>
-        <v>524</v>
+        <v>427</v>
       </c>
     </row>
     <row r="32" spans="2:24">
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="77" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="75"/>
-      <c r="D32" s="75"/>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75"/>
-      <c r="I32" s="75"/>
-      <c r="J32" s="75"/>
-      <c r="K32" s="75"/>
-      <c r="L32" s="75"/>
-      <c r="M32" s="75"/>
-      <c r="N32" s="75"/>
-      <c r="O32" s="75"/>
-      <c r="P32" s="75"/>
-      <c r="Q32" s="75"/>
-      <c r="R32" s="75"/>
-      <c r="S32" s="75"/>
-      <c r="T32" s="75"/>
-      <c r="U32" s="75"/>
-      <c r="V32" s="75"/>
-      <c r="W32" s="75"/>
-      <c r="X32" s="75"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="77"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="77"/>
+      <c r="L32" s="77"/>
+      <c r="M32" s="77"/>
+      <c r="N32" s="77"/>
+      <c r="O32" s="77"/>
+      <c r="P32" s="77"/>
+      <c r="Q32" s="77"/>
+      <c r="R32" s="77"/>
+      <c r="S32" s="77"/>
+      <c r="T32" s="77"/>
+      <c r="U32" s="77"/>
+      <c r="V32" s="77"/>
+      <c r="W32" s="77"/>
+      <c r="X32" s="77"/>
     </row>
     <row r="33" spans="2:25" ht="27.75" customHeight="1">
       <c r="B33" s="11" t="s">
@@ -4163,7 +4574,7 @@
       </c>
     </row>
     <row r="34" spans="2:25">
-      <c r="B34" s="66" t="s">
+      <c r="B34" s="68" t="s">
         <v>47</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -4240,7 +4651,7 @@
       </c>
     </row>
     <row r="35" spans="2:25">
-      <c r="B35" s="66"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="2" t="s">
         <v>45</v>
       </c>
@@ -4314,7 +4725,7 @@
       </c>
     </row>
     <row r="36" spans="2:25">
-      <c r="B36" s="66"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="21" t="s">
         <v>46</v>
       </c>
@@ -4404,7 +4815,7 @@
       </c>
     </row>
     <row r="37" spans="2:25">
-      <c r="B37" s="66" t="s">
+      <c r="B37" s="68" t="s">
         <v>50</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -4481,7 +4892,7 @@
       </c>
     </row>
     <row r="38" spans="2:25">
-      <c r="B38" s="66"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="2" t="s">
         <v>78</v>
       </c>
@@ -4556,7 +4967,7 @@
       </c>
     </row>
     <row r="39" spans="2:25">
-      <c r="B39" s="66"/>
+      <c r="B39" s="68"/>
       <c r="C39" s="21" t="s">
         <v>51</v>
       </c>
@@ -4646,7 +5057,7 @@
       </c>
     </row>
     <row r="40" spans="2:25">
-      <c r="B40" s="66" t="s">
+      <c r="B40" s="68" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -4723,7 +5134,7 @@
       </c>
     </row>
     <row r="41" spans="2:25">
-      <c r="B41" s="66"/>
+      <c r="B41" s="68"/>
       <c r="C41" s="2" t="s">
         <v>53</v>
       </c>
@@ -4798,7 +5209,7 @@
       </c>
     </row>
     <row r="42" spans="2:25">
-      <c r="B42" s="66"/>
+      <c r="B42" s="68"/>
       <c r="C42" s="21" t="s">
         <v>54</v>
       </c>
@@ -4977,54 +5388,54 @@
       </c>
     </row>
     <row r="47" spans="2:25">
-      <c r="B47" s="70" t="s">
+      <c r="B47" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="C47" s="70"/>
-      <c r="D47" s="70"/>
-      <c r="E47" s="70"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="72"/>
+      <c r="E47" s="72"/>
     </row>
     <row r="48" spans="2:25" ht="27.75" customHeight="1">
-      <c r="B48" s="69" t="s">
+      <c r="B48" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="C48" s="69"/>
+      <c r="C48" s="71"/>
       <c r="D48" s="22" t="s">
         <v>71</v>
       </c>
       <c r="E48" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="G48" s="65" t="s">
+      <c r="G48" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="H48" s="65"/>
-      <c r="J48" s="65" t="s">
+      <c r="H48" s="67"/>
+      <c r="J48" s="67" t="s">
         <v>79</v>
       </c>
-      <c r="K48" s="65"/>
-      <c r="L48" s="65"/>
+      <c r="K48" s="67"/>
+      <c r="L48" s="67"/>
       <c r="N48" s="30" t="s">
         <v>97</v>
       </c>
       <c r="O48" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="Q48" s="68" t="s">
+      <c r="Q48" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="R48" s="68"/>
-      <c r="S48" s="68"/>
-      <c r="T48" s="68"/>
-      <c r="U48" s="68"/>
-      <c r="W48" s="64" t="s">
+      <c r="R48" s="70"/>
+      <c r="S48" s="70"/>
+      <c r="T48" s="70"/>
+      <c r="U48" s="70"/>
+      <c r="W48" s="66" t="s">
         <v>114</v>
       </c>
-      <c r="X48" s="64"/>
-      <c r="Y48" s="64"/>
+      <c r="X48" s="66"/>
+      <c r="Y48" s="66"/>
     </row>
     <row r="49" spans="2:25">
-      <c r="B49" s="69" t="s">
+      <c r="B49" s="71" t="s">
         <v>69</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -5058,19 +5469,19 @@
       <c r="O49" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="Q49" s="66" t="s">
+      <c r="Q49" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="R49" s="67" t="s">
+      <c r="R49" s="69" t="s">
         <v>102</v>
       </c>
-      <c r="S49" s="67" t="s">
+      <c r="S49" s="69" t="s">
         <v>103</v>
       </c>
-      <c r="T49" s="67" t="s">
+      <c r="T49" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="U49" s="67"/>
+      <c r="U49" s="69"/>
       <c r="W49" s="34" t="s">
         <v>115</v>
       </c>
@@ -5082,7 +5493,7 @@
       </c>
     </row>
     <row r="50" spans="2:25">
-      <c r="B50" s="69"/>
+      <c r="B50" s="71"/>
       <c r="C50" s="2" t="s">
         <v>58</v>
       </c>
@@ -5115,9 +5526,9 @@
       <c r="O50" s="2">
         <v>8</v>
       </c>
-      <c r="Q50" s="66"/>
-      <c r="R50" s="67"/>
-      <c r="S50" s="67"/>
+      <c r="Q50" s="68"/>
+      <c r="R50" s="69"/>
+      <c r="S50" s="69"/>
       <c r="T50" s="10" t="s">
         <v>104</v>
       </c>
@@ -5136,7 +5547,7 @@
       </c>
     </row>
     <row r="51" spans="2:25">
-      <c r="B51" s="69"/>
+      <c r="B51" s="71"/>
       <c r="C51" s="2" t="s">
         <v>59</v>
       </c>
@@ -5193,7 +5604,7 @@
       </c>
     </row>
     <row r="52" spans="2:25">
-      <c r="B52" s="69"/>
+      <c r="B52" s="71"/>
       <c r="C52" s="2" t="s">
         <v>60</v>
       </c>
@@ -5249,7 +5660,7 @@
       </c>
     </row>
     <row r="53" spans="2:25">
-      <c r="B53" s="69"/>
+      <c r="B53" s="71"/>
       <c r="C53" s="2" t="s">
         <v>61</v>
       </c>
@@ -5299,14 +5710,14 @@
       </c>
     </row>
     <row r="54" spans="2:25">
-      <c r="B54" s="69"/>
+      <c r="B54" s="71"/>
       <c r="C54" s="2" t="s">
         <v>62</v>
       </c>
       <c r="D54" s="4">
         <v>0.01</v>
       </c>
-      <c r="E54" s="111">
+      <c r="E54" s="113">
         <f t="shared" si="9"/>
         <v>7377.17</v>
       </c>
@@ -5339,7 +5750,7 @@
       </c>
     </row>
     <row r="55" spans="2:25">
-      <c r="B55" s="69" t="s">
+      <c r="B55" s="71" t="s">
         <v>70</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -5378,7 +5789,7 @@
       </c>
     </row>
     <row r="56" spans="2:25">
-      <c r="B56" s="69"/>
+      <c r="B56" s="71"/>
       <c r="C56" s="2" t="s">
         <v>64</v>
       </c>
@@ -5401,7 +5812,7 @@
       </c>
     </row>
     <row r="57" spans="2:25">
-      <c r="B57" s="69"/>
+      <c r="B57" s="71"/>
       <c r="C57" s="2" t="s">
         <v>65</v>
       </c>
@@ -5424,7 +5835,7 @@
       </c>
     </row>
     <row r="58" spans="2:25">
-      <c r="B58" s="69"/>
+      <c r="B58" s="71"/>
       <c r="C58" s="2" t="s">
         <v>66</v>
       </c>
@@ -5483,10 +5894,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:L102"/>
+  <dimension ref="A2:T186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B106" sqref="B106"/>
+    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
+      <selection activeCell="B185" sqref="B185:F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5496,35 +5907,39 @@
     <col min="4" max="4" width="18.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="19.140625" customWidth="1"/>
     <col min="10" max="10" width="21.28515625" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16" customWidth="1"/>
+    <col min="15" max="15" width="18.140625" customWidth="1"/>
+    <col min="16" max="17" width="15.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12">
-      <c r="H2" s="99" t="s">
+      <c r="H2" s="101" t="s">
         <v>147</v>
       </c>
-      <c r="I2" s="100"/>
-      <c r="J2" s="100"/>
-      <c r="K2" s="100"/>
-      <c r="L2" s="100"/>
+      <c r="I2" s="102"/>
+      <c r="J2" s="102"/>
+      <c r="K2" s="102"/>
+      <c r="L2" s="102"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="B3" s="88" t="s">
+      <c r="B3" s="90" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="H3" s="97" t="s">
+      <c r="C3" s="90"/>
+      <c r="D3" s="90"/>
+      <c r="E3" s="90"/>
+      <c r="F3" s="90"/>
+      <c r="H3" s="99" t="s">
         <v>68</v>
       </c>
-      <c r="I3" s="97"/>
-      <c r="J3" s="97"/>
+      <c r="I3" s="99"/>
+      <c r="J3" s="99"/>
       <c r="K3" s="2" t="s">
         <v>81</v>
       </c>
@@ -5548,11 +5963,11 @@
       <c r="F4" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="99" t="s">
         <v>138</v>
       </c>
-      <c r="I4" s="97"/>
-      <c r="J4" s="97"/>
+      <c r="I4" s="99"/>
+      <c r="J4" s="99"/>
       <c r="K4" s="40">
         <v>0</v>
       </c>
@@ -5579,11 +5994,11 @@
         <f>E5/$E$16</f>
         <v>0.69059405940594054</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="99" t="s">
         <v>139</v>
       </c>
-      <c r="I5" s="97"/>
-      <c r="J5" s="97"/>
+      <c r="I5" s="99"/>
+      <c r="J5" s="99"/>
       <c r="K5" s="40">
         <v>51000</v>
       </c>
@@ -5597,14 +6012,14 @@
         <v>130</v>
       </c>
       <c r="C6" s="10"/>
-      <c r="D6" s="112"/>
+      <c r="D6" s="114"/>
       <c r="E6" s="27"/>
       <c r="F6" s="3"/>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="99" t="s">
         <v>140</v>
       </c>
-      <c r="I6" s="97"/>
-      <c r="J6" s="97"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
       <c r="K6" s="40">
         <v>0</v>
       </c>
@@ -5679,11 +6094,11 @@
       <c r="D9" s="27"/>
       <c r="E9" s="27"/>
       <c r="F9" s="3"/>
-      <c r="H9" s="102" t="s">
+      <c r="H9" s="104" t="s">
         <v>143</v>
       </c>
-      <c r="I9" s="102"/>
-      <c r="J9" s="102"/>
+      <c r="I9" s="104"/>
+      <c r="J9" s="104"/>
       <c r="K9" s="40">
         <v>0</v>
       </c>
@@ -5708,11 +6123,11 @@
       <c r="F10" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="99" t="s">
         <v>144</v>
       </c>
-      <c r="I10" s="97"/>
-      <c r="J10" s="97"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="99"/>
       <c r="K10" s="40">
         <v>0</v>
       </c>
@@ -5734,11 +6149,11 @@
         <f>E11/$E$16</f>
         <v>0</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="99" t="s">
         <v>145</v>
       </c>
-      <c r="I11" s="97"/>
-      <c r="J11" s="97"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="99"/>
       <c r="K11" s="40">
         <v>0</v>
       </c>
@@ -5755,11 +6170,11 @@
       <c r="D12" s="27"/>
       <c r="E12" s="27"/>
       <c r="F12" s="3"/>
-      <c r="H12" s="98" t="s">
+      <c r="H12" s="100" t="s">
         <v>146</v>
       </c>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
+      <c r="I12" s="100"/>
+      <c r="J12" s="100"/>
       <c r="K12" s="42">
         <f>SUM(K4:K11)</f>
         <v>640000</v>
@@ -5818,11 +6233,11 @@
       </c>
     </row>
     <row r="16" spans="2:12">
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="105" t="s">
         <v>137</v>
       </c>
-      <c r="C16" s="104"/>
-      <c r="D16" s="104"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
       <c r="E16" s="37">
         <f>E5+E8+E11+E15</f>
         <v>4848000</v>
@@ -5837,10 +6252,10 @@
       <c r="E17" s="16"/>
     </row>
     <row r="18" spans="2:12">
-      <c r="B18" s="106" t="s">
+      <c r="B18" s="108" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="106"/>
+      <c r="C18" s="108"/>
       <c r="D18" s="16"/>
       <c r="E18" s="16"/>
     </row>
@@ -5878,49 +6293,49 @@
       <c r="E21" s="16"/>
     </row>
     <row r="23" spans="2:12">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="89" t="s">
         <v>161</v>
       </c>
-      <c r="C23" s="87"/>
-      <c r="D23" s="87"/>
-      <c r="E23" s="87"/>
-      <c r="F23" s="87"/>
-      <c r="G23" s="87"/>
-      <c r="H23" s="87"/>
-      <c r="I23" s="87"/>
-      <c r="J23" s="87"/>
+      <c r="C23" s="89"/>
+      <c r="D23" s="89"/>
+      <c r="E23" s="89"/>
+      <c r="F23" s="89"/>
+      <c r="G23" s="89"/>
+      <c r="H23" s="89"/>
+      <c r="I23" s="89"/>
+      <c r="J23" s="89"/>
     </row>
     <row r="24" spans="2:12">
-      <c r="B24" s="67" t="s">
+      <c r="B24" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="C24" s="67" t="s">
+      <c r="C24" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="D24" s="67" t="s">
+      <c r="D24" s="69" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="67" t="s">
+      <c r="E24" s="69" t="s">
         <v>152</v>
       </c>
-      <c r="F24" s="67" t="s">
+      <c r="F24" s="69" t="s">
         <v>153</v>
       </c>
-      <c r="G24" s="101" t="s">
+      <c r="G24" s="103" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="67" t="s">
+      <c r="H24" s="103"/>
+      <c r="I24" s="103"/>
+      <c r="J24" s="69" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:12">
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
       <c r="G25" s="2" t="s">
         <v>2</v>
       </c>
@@ -5930,7 +6345,7 @@
       <c r="I25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="67"/>
+      <c r="J25" s="69"/>
     </row>
     <row r="26" spans="2:12">
       <c r="B26" s="22" t="s">
@@ -5978,22 +6393,22 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="15" customHeight="1">
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="93" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="92"/>
-      <c r="D28" s="92"/>
-      <c r="E28" s="92"/>
-      <c r="F28" s="93"/>
-      <c r="G28" s="60">
+      <c r="C28" s="94"/>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="95"/>
+      <c r="G28" s="63">
         <f>G27</f>
         <v>200000</v>
       </c>
-      <c r="H28" s="60">
+      <c r="H28" s="63">
         <f t="shared" ref="H28:I28" si="1">H27</f>
         <v>200000</v>
       </c>
-      <c r="I28" s="60">
+      <c r="I28" s="63">
         <f t="shared" si="1"/>
         <v>200000</v>
       </c>
@@ -6018,14 +6433,14 @@
       <c r="F29" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G29" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="I29" s="35" t="s">
-        <v>136</v>
+      <c r="G29" s="35">
+        <v>0</v>
+      </c>
+      <c r="H29" s="35">
+        <v>0</v>
+      </c>
+      <c r="I29" s="35">
+        <v>0</v>
       </c>
       <c r="J29" s="48" t="s">
         <v>160</v>
@@ -6047,35 +6462,38 @@
       <c r="F30" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="G30" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="H30" s="35" t="s">
-        <v>136</v>
-      </c>
-      <c r="I30" s="35" t="s">
-        <v>136</v>
+      <c r="G30" s="35">
+        <v>0</v>
+      </c>
+      <c r="H30" s="35">
+        <v>0</v>
+      </c>
+      <c r="I30" s="35">
+        <v>0</v>
       </c>
       <c r="J30" s="48" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="31" spans="2:12">
-      <c r="B31" s="94" t="s">
+      <c r="B31" s="96" t="s">
         <v>159</v>
       </c>
-      <c r="C31" s="95"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="95"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="61">
-        <v>0</v>
-      </c>
-      <c r="H31" s="61">
-        <v>0</v>
-      </c>
-      <c r="I31" s="61">
-        <v>0</v>
+      <c r="C31" s="97"/>
+      <c r="D31" s="97"/>
+      <c r="E31" s="97"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="123">
+        <f>G28+G30+G29</f>
+        <v>200000</v>
+      </c>
+      <c r="H31" s="123">
+        <f t="shared" ref="H31:I31" si="2">H28+H30+H29</f>
+        <v>200000</v>
+      </c>
+      <c r="I31" s="123">
+        <f t="shared" si="2"/>
+        <v>200000</v>
       </c>
       <c r="J31" s="37">
         <f>SUM(J28:J30)</f>
@@ -6087,35 +6505,35 @@
       <c r="L31" s="17"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="89" t="s">
         <v>167</v>
       </c>
-      <c r="C33" s="87"/>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="87"/>
+      <c r="C33" s="89"/>
+      <c r="D33" s="89"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="89"/>
+      <c r="G33" s="89"/>
     </row>
     <row r="34" spans="2:7">
-      <c r="B34" s="67" t="s">
+      <c r="B34" s="69" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="67" t="s">
+      <c r="C34" s="69" t="s">
         <v>164</v>
       </c>
-      <c r="D34" s="67" t="s">
+      <c r="D34" s="69" t="s">
         <v>165</v>
       </c>
-      <c r="E34" s="67" t="s">
+      <c r="E34" s="69" t="s">
         <v>166</v>
       </c>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
     </row>
     <row r="35" spans="2:7">
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
+      <c r="B35" s="69"/>
+      <c r="C35" s="69"/>
+      <c r="D35" s="69"/>
       <c r="E35" s="10" t="s">
         <v>2</v>
       </c>
@@ -6151,12 +6569,12 @@
       </c>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="87" t="s">
+      <c r="B38" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="C38" s="87"/>
-      <c r="D38" s="87"/>
-      <c r="E38" s="87"/>
+      <c r="C38" s="89"/>
+      <c r="D38" s="89"/>
+      <c r="E38" s="89"/>
     </row>
     <row r="39" spans="2:7">
       <c r="B39" s="51" t="s">
@@ -6217,12 +6635,12 @@
       <c r="E43" s="1"/>
     </row>
     <row r="44" spans="2:7">
-      <c r="B44" s="87" t="s">
+      <c r="B44" s="89" t="s">
         <v>175</v>
       </c>
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="F44" s="88" t="s">
+      <c r="C44" s="89"/>
+      <c r="D44" s="89"/>
+      <c r="F44" s="90" t="s">
         <v>176</v>
       </c>
     </row>
@@ -6236,7 +6654,7 @@
       <c r="D45" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="F45" s="88"/>
+      <c r="F45" s="90"/>
     </row>
     <row r="46" spans="2:7">
       <c r="B46" s="2" t="s">
@@ -6250,7 +6668,7 @@
         <f>C46*'Demanda Dinamica'!$L$50*'Demanda Dinamica'!F37</f>
         <v>606666.66666666663</v>
       </c>
-      <c r="F46" s="88"/>
+      <c r="F46" s="90"/>
     </row>
     <row r="47" spans="2:7">
       <c r="B47" s="2" t="s">
@@ -6311,20 +6729,20 @@
       <c r="D51" s="9"/>
     </row>
     <row r="52" spans="2:7">
-      <c r="B52" s="90" t="s">
+      <c r="B52" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="C52" s="90"/>
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="90"/>
-      <c r="G52" s="90"/>
+      <c r="C52" s="92"/>
+      <c r="D52" s="92"/>
+      <c r="E52" s="92"/>
+      <c r="F52" s="92"/>
+      <c r="G52" s="92"/>
     </row>
     <row r="53" spans="2:7">
-      <c r="B53" s="89" t="s">
+      <c r="B53" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="C53" s="89"/>
+      <c r="C53" s="91"/>
       <c r="D53" s="22" t="s">
         <v>177</v>
       </c>
@@ -6339,10 +6757,10 @@
       </c>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="79" t="s">
         <v>178</v>
       </c>
-      <c r="C54" s="77"/>
+      <c r="C54" s="79"/>
       <c r="D54" s="18">
         <f>E16</f>
         <v>4848000</v>
@@ -6361,10 +6779,10 @@
       </c>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="77" t="s">
+      <c r="B55" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="C55" s="77"/>
+      <c r="C55" s="79"/>
       <c r="D55" s="18">
         <v>0</v>
       </c>
@@ -6381,10 +6799,10 @@
       </c>
     </row>
     <row r="56" spans="2:7">
-      <c r="B56" s="77" t="s">
+      <c r="B56" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="C56" s="77"/>
+      <c r="C56" s="79"/>
       <c r="D56" s="18">
         <v>10000</v>
       </c>
@@ -6402,10 +6820,10 @@
       </c>
     </row>
     <row r="57" spans="2:7">
-      <c r="B57" s="77" t="s">
+      <c r="B57" s="79" t="s">
         <v>181</v>
       </c>
-      <c r="C57" s="77"/>
+      <c r="C57" s="79"/>
       <c r="D57" s="18">
         <v>0</v>
       </c>
@@ -6420,10 +6838,10 @@
       </c>
     </row>
     <row r="58" spans="2:7">
-      <c r="B58" s="77" t="s">
+      <c r="B58" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="C58" s="77"/>
+      <c r="C58" s="79"/>
       <c r="D58" s="18">
         <v>0</v>
       </c>
@@ -6438,10 +6856,10 @@
       </c>
     </row>
     <row r="59" spans="2:7">
-      <c r="B59" s="77" t="s">
+      <c r="B59" s="79" t="s">
         <v>183</v>
       </c>
-      <c r="C59" s="77"/>
+      <c r="C59" s="79"/>
       <c r="D59" s="18">
         <v>0</v>
       </c>
@@ -6456,40 +6874,40 @@
       </c>
     </row>
     <row r="60" spans="2:7">
-      <c r="B60" s="85" t="s">
+      <c r="B60" s="87" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="85"/>
-      <c r="D60" s="85"/>
+      <c r="C60" s="87"/>
+      <c r="D60" s="87"/>
       <c r="E60" s="25">
         <f>SUM(E54:E59)</f>
         <v>168480</v>
       </c>
       <c r="F60" s="25">
-        <f t="shared" ref="F60:G60" si="2">SUM(F54:F59)</f>
+        <f t="shared" ref="F60:G60" si="3">SUM(F54:F59)</f>
         <v>178588.79999999999</v>
       </c>
       <c r="G60" s="25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>190197.07199999999</v>
       </c>
     </row>
     <row r="62" spans="2:7">
-      <c r="B62" s="105" t="s">
+      <c r="B62" s="107" t="s">
         <v>200</v>
       </c>
-      <c r="C62" s="105"/>
-      <c r="D62" s="105"/>
-      <c r="E62" s="105"/>
-      <c r="F62" s="105"/>
-      <c r="G62" s="105"/>
+      <c r="C62" s="107"/>
+      <c r="D62" s="107"/>
+      <c r="E62" s="107"/>
+      <c r="F62" s="107"/>
+      <c r="G62" s="107"/>
     </row>
     <row r="63" spans="2:7">
-      <c r="B63" s="69" t="s">
+      <c r="B63" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="C63" s="69"/>
-      <c r="D63" s="69"/>
+      <c r="C63" s="71"/>
+      <c r="D63" s="71"/>
       <c r="E63" s="22" t="s">
         <v>2</v>
       </c>
@@ -6501,13 +6919,13 @@
       </c>
     </row>
     <row r="64" spans="2:7">
-      <c r="B64" s="86" t="s">
+      <c r="B64" s="88" t="s">
         <v>194</v>
       </c>
-      <c r="C64" s="77" t="s">
+      <c r="C64" s="79" t="s">
         <v>186</v>
       </c>
-      <c r="D64" s="77"/>
+      <c r="D64" s="79"/>
       <c r="E64" s="19">
         <f>0</f>
         <v>0</v>
@@ -6522,11 +6940,11 @@
       </c>
     </row>
     <row r="65" spans="2:8">
-      <c r="B65" s="86"/>
-      <c r="C65" s="77" t="s">
+      <c r="B65" s="88"/>
+      <c r="C65" s="79" t="s">
         <v>198</v>
       </c>
-      <c r="D65" s="77"/>
+      <c r="D65" s="79"/>
       <c r="E65" s="19">
         <f>'Demanda Dinamica'!V39</f>
         <v>24963480</v>
@@ -6541,11 +6959,11 @@
       </c>
     </row>
     <row r="66" spans="2:8">
-      <c r="B66" s="86"/>
-      <c r="C66" s="77" t="s">
+      <c r="B66" s="88"/>
+      <c r="C66" s="79" t="s">
         <v>197</v>
       </c>
-      <c r="D66" s="77"/>
+      <c r="D66" s="79"/>
       <c r="E66" s="19">
         <f>'Demanda Dinamica'!$V$42</f>
         <v>4109020</v>
@@ -6560,11 +6978,11 @@
       </c>
     </row>
     <row r="67" spans="2:8">
-      <c r="B67" s="86"/>
-      <c r="C67" s="77" t="s">
+      <c r="B67" s="88"/>
+      <c r="C67" s="79" t="s">
         <v>199</v>
       </c>
-      <c r="D67" s="77"/>
+      <c r="D67" s="79"/>
       <c r="E67" s="19">
         <f>'Demanda Dinamica'!V36</f>
         <v>16262030</v>
@@ -6579,11 +6997,11 @@
       </c>
     </row>
     <row r="68" spans="2:8">
-      <c r="B68" s="86"/>
-      <c r="C68" s="77" t="s">
+      <c r="B68" s="88"/>
+      <c r="C68" s="79" t="s">
         <v>187</v>
       </c>
-      <c r="D68" s="77"/>
+      <c r="D68" s="79"/>
       <c r="E68" s="19">
         <v>0</v>
       </c>
@@ -6597,35 +7015,35 @@
       </c>
     </row>
     <row r="69" spans="2:8">
-      <c r="B69" s="86"/>
-      <c r="C69" s="82" t="s">
+      <c r="B69" s="88"/>
+      <c r="C69" s="84" t="s">
         <v>188</v>
       </c>
-      <c r="D69" s="82"/>
+      <c r="D69" s="84"/>
       <c r="E69" s="58">
         <f>SUM(E64:E67)-E68</f>
         <v>45334530</v>
       </c>
       <c r="F69" s="58">
-        <f t="shared" ref="F69:G69" si="3">SUM(F64:F67)-F68</f>
+        <f t="shared" ref="F69:G69" si="4">SUM(F64:F67)-F68</f>
         <v>48054601.799999997</v>
       </c>
       <c r="G69" s="58">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>48281274.450000003</v>
       </c>
-      <c r="H69" s="62" t="s">
+      <c r="H69" s="64" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="70" spans="2:8">
-      <c r="B70" s="86" t="s">
+      <c r="B70" s="88" t="s">
         <v>195</v>
       </c>
-      <c r="C70" s="77" t="s">
+      <c r="C70" s="79" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="77"/>
+      <c r="D70" s="79"/>
       <c r="E70" s="19">
         <v>0</v>
       </c>
@@ -6641,11 +7059,11 @@
       </c>
     </row>
     <row r="71" spans="2:8">
-      <c r="B71" s="86"/>
-      <c r="C71" s="77" t="s">
+      <c r="B71" s="88"/>
+      <c r="C71" s="79" t="s">
         <v>190</v>
       </c>
-      <c r="D71" s="77"/>
+      <c r="D71" s="79"/>
       <c r="E71" s="19">
         <f>G28</f>
         <v>200000</v>
@@ -6659,16 +7077,16 @@
         <v>213000</v>
       </c>
       <c r="H71" s="19">
-        <f t="shared" ref="H71:H73" si="4">E71/12</f>
+        <f t="shared" ref="H71:H73" si="5">E71/12</f>
         <v>16666.666666666668</v>
       </c>
     </row>
     <row r="72" spans="2:8">
-      <c r="B72" s="86"/>
-      <c r="C72" s="77" t="s">
+      <c r="B72" s="88"/>
+      <c r="C72" s="79" t="s">
         <v>191</v>
       </c>
-      <c r="D72" s="77"/>
+      <c r="D72" s="79"/>
       <c r="E72" s="19">
         <v>0</v>
       </c>
@@ -6679,16 +7097,16 @@
         <v>0</v>
       </c>
       <c r="H72" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="73" spans="2:8">
-      <c r="B73" s="86"/>
-      <c r="C73" s="77" t="s">
+      <c r="B73" s="88"/>
+      <c r="C73" s="79" t="s">
         <v>192</v>
       </c>
-      <c r="D73" s="77"/>
+      <c r="D73" s="79"/>
       <c r="E73" s="19">
         <v>0</v>
       </c>
@@ -6699,54 +7117,54 @@
         <v>0</v>
       </c>
       <c r="H73" s="19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:8">
-      <c r="B74" s="86"/>
-      <c r="C74" s="82" t="s">
+      <c r="B74" s="88"/>
+      <c r="C74" s="84" t="s">
         <v>193</v>
       </c>
-      <c r="D74" s="82"/>
+      <c r="D74" s="84"/>
       <c r="E74" s="58">
         <f xml:space="preserve"> SUM(E70:E73)</f>
         <v>200000</v>
       </c>
       <c r="F74" s="58">
-        <f t="shared" ref="F74:G74" si="5" xml:space="preserve"> SUM(F70:F73)</f>
+        <f t="shared" ref="F74:G74" si="6" xml:space="preserve"> SUM(F70:F73)</f>
         <v>212000</v>
       </c>
       <c r="G74" s="58">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>213000</v>
       </c>
     </row>
     <row r="75" spans="2:8">
-      <c r="B75" s="85" t="s">
+      <c r="B75" s="87" t="s">
         <v>196</v>
       </c>
-      <c r="C75" s="85"/>
-      <c r="D75" s="85"/>
+      <c r="C75" s="87"/>
+      <c r="D75" s="87"/>
       <c r="E75" s="58">
         <f>E69+E74</f>
         <v>45534530</v>
       </c>
       <c r="F75" s="58">
-        <f t="shared" ref="F75:G75" si="6">F69+F74</f>
+        <f t="shared" ref="F75:G75" si="7">F69+F74</f>
         <v>48266601.799999997</v>
       </c>
       <c r="G75" s="58">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>48494274.450000003</v>
       </c>
     </row>
     <row r="78" spans="2:8">
-      <c r="B78" s="82" t="s">
+      <c r="B78" s="84" t="s">
         <v>202</v>
       </c>
-      <c r="C78" s="82"/>
-      <c r="D78" s="82"/>
+      <c r="C78" s="84"/>
+      <c r="D78" s="84"/>
       <c r="E78" s="58">
         <f>E75/('Demanda Dinamica'!$Y$52*12)</f>
         <v>3162.120138888889</v>
@@ -6761,23 +7179,23 @@
       </c>
     </row>
     <row r="81" spans="2:7">
-      <c r="B81" s="83" t="s">
+      <c r="B81" s="85" t="s">
         <v>203</v>
       </c>
-      <c r="C81" s="83"/>
+      <c r="C81" s="85"/>
       <c r="D81" s="4">
         <v>0.35</v>
       </c>
-      <c r="F81" s="83" t="s">
+      <c r="F81" s="85" t="s">
         <v>206</v>
       </c>
-      <c r="G81" s="83"/>
+      <c r="G81" s="85"/>
     </row>
     <row r="82" spans="2:7">
-      <c r="B82" s="83" t="s">
+      <c r="B82" s="85" t="s">
         <v>204</v>
       </c>
-      <c r="C82" s="83"/>
+      <c r="C82" s="85"/>
       <c r="D82" s="19">
         <f>E78*D81</f>
         <v>1106.7420486111112</v>
@@ -6791,11 +7209,11 @@
       </c>
     </row>
     <row r="83" spans="2:7">
-      <c r="B83" s="84" t="s">
+      <c r="B83" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="C83" s="84"/>
-      <c r="D83" s="63">
+      <c r="C83" s="86"/>
+      <c r="D83" s="65">
         <f>E78*(1+D81)</f>
         <v>4268.8621875000008</v>
       </c>
@@ -6835,11 +7253,11 @@
       </c>
     </row>
     <row r="89" spans="2:7">
-      <c r="B89" s="85" t="s">
+      <c r="B89" s="87" t="s">
         <v>211</v>
       </c>
-      <c r="C89" s="85"/>
-      <c r="D89" s="85"/>
+      <c r="C89" s="87"/>
+      <c r="D89" s="87"/>
       <c r="E89" s="58">
         <f>E78+G86</f>
         <v>4016.063330876389</v>
@@ -6854,65 +7272,65 @@
       </c>
     </row>
     <row r="92" spans="2:7">
-      <c r="B92" s="107" t="s">
+      <c r="B92" s="109" t="s">
         <v>212</v>
       </c>
-      <c r="C92" s="107"/>
-      <c r="D92" s="108">
+      <c r="C92" s="109"/>
+      <c r="D92" s="110">
         <f>+(D83-E89)/D83</f>
         <v>5.9219259259259402E-2</v>
       </c>
     </row>
     <row r="93" spans="2:7">
-      <c r="B93" s="107" t="s">
+      <c r="B93" s="109" t="s">
         <v>213</v>
       </c>
-      <c r="C93" s="107"/>
-      <c r="D93" s="109">
+      <c r="C93" s="109"/>
+      <c r="D93" s="111">
         <f>E89*D92</f>
         <v>237.82829559277377</v>
       </c>
     </row>
     <row r="95" spans="2:7">
-      <c r="B95" s="113" t="s">
+      <c r="B95" s="115" t="s">
         <v>214</v>
       </c>
-      <c r="C95" s="113"/>
-      <c r="D95" s="113"/>
-      <c r="E95" s="113"/>
+      <c r="C95" s="115"/>
+      <c r="D95" s="115"/>
+      <c r="E95" s="115"/>
     </row>
     <row r="96" spans="2:7">
-      <c r="B96" s="59" t="s">
+      <c r="B96" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="C96" s="59" t="s">
+      <c r="C96" s="60" t="s">
         <v>219</v>
       </c>
-      <c r="D96" s="59" t="s">
+      <c r="D96" s="60" t="s">
         <v>220</v>
       </c>
-      <c r="E96" s="59" t="s">
+      <c r="E96" s="60" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="97" spans="2:5">
+    <row r="97" spans="2:7">
       <c r="B97" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C97" s="114">
+      <c r="C97" s="116">
         <f>'Demanda Dinamica'!V43</f>
         <v>45334530</v>
       </c>
-      <c r="D97" s="114">
+      <c r="D97" s="116">
         <f>'Demanda Dinamica'!W43</f>
         <v>48054601.800000004</v>
       </c>
-      <c r="E97" s="114">
+      <c r="E97" s="116">
         <f>'Demanda Dinamica'!X43</f>
         <v>51178150.917000011</v>
       </c>
     </row>
-    <row r="98" spans="2:5">
+    <row r="98" spans="2:7">
       <c r="B98" s="2" t="s">
         <v>223</v>
       </c>
@@ -6921,15 +7339,15 @@
         <v>45534530</v>
       </c>
       <c r="D98" s="19">
-        <f t="shared" ref="D98:E98" si="7">F75</f>
+        <f t="shared" ref="D98:E98" si="8">F75</f>
         <v>48266601.799999997</v>
       </c>
       <c r="E98" s="19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>48494274.450000003</v>
       </c>
     </row>
-    <row r="99" spans="2:5">
+    <row r="99" spans="2:7">
       <c r="B99" s="2" t="s">
         <v>224</v>
       </c>
@@ -6938,37 +7356,2077 @@
         <v>168480</v>
       </c>
       <c r="D99" s="18">
-        <f t="shared" ref="D99:E99" si="8">F60</f>
+        <f t="shared" ref="D99:E99" si="9">F60</f>
         <v>178588.79999999999</v>
       </c>
       <c r="E99" s="18">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>190197.07199999999</v>
       </c>
     </row>
-    <row r="100" spans="2:5">
+    <row r="100" spans="2:7">
       <c r="B100" s="21" t="s">
         <v>225</v>
       </c>
-      <c r="C100" s="115">
+      <c r="C100" s="117">
         <f>SUM(C97:C99)</f>
         <v>91037540</v>
       </c>
-      <c r="D100" s="115">
-        <f t="shared" ref="D100:E100" si="9">SUM(D97:D99)</f>
+      <c r="D100" s="117">
+        <f t="shared" ref="D100:E100" si="10">SUM(D97:D99)</f>
         <v>96499792.399999991</v>
       </c>
-      <c r="E100" s="115">
-        <f t="shared" si="9"/>
+      <c r="E100" s="117">
+        <f t="shared" si="10"/>
         <v>99862622.43900001</v>
       </c>
     </row>
-    <row r="102" spans="2:5">
-      <c r="B102" s="116"/>
+    <row r="102" spans="2:7">
+      <c r="B102" s="118"/>
+    </row>
+    <row r="103" spans="2:7">
+      <c r="B103" s="119" t="s">
+        <v>226</v>
+      </c>
+      <c r="C103" s="119"/>
+      <c r="D103" s="119"/>
+      <c r="E103" s="119"/>
+      <c r="F103" s="119"/>
+      <c r="G103" s="119"/>
+    </row>
+    <row r="104" spans="2:7">
+      <c r="B104" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="C104" s="71"/>
+      <c r="D104" s="62" t="s">
+        <v>236</v>
+      </c>
+      <c r="E104" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F104" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="G104" s="62" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="105" spans="2:7">
+      <c r="B105" s="104" t="s">
+        <v>227</v>
+      </c>
+      <c r="C105" s="104"/>
+      <c r="D105" s="121">
+        <f>'Demanda Dinamica'!I36</f>
+        <v>2180290</v>
+      </c>
+      <c r="E105" s="121">
+        <f>'Demanda Dinamica'!V36</f>
+        <v>16262030</v>
+      </c>
+      <c r="F105" s="121">
+        <f>'Demanda Dinamica'!W36</f>
+        <v>17237751.800000001</v>
+      </c>
+      <c r="G105" s="121">
+        <f>'Demanda Dinamica'!X36</f>
+        <v>18358205.667000003</v>
+      </c>
+    </row>
+    <row r="106" spans="2:7">
+      <c r="B106" s="104" t="s">
+        <v>178</v>
+      </c>
+      <c r="C106" s="104"/>
+      <c r="D106" s="121">
+        <f>E16</f>
+        <v>4848000</v>
+      </c>
+      <c r="E106" s="122">
+        <f>D106*1%</f>
+        <v>48480</v>
+      </c>
+      <c r="F106" s="121">
+        <f>E106*(1+'Demanda Dinamica'!$D$6)</f>
+        <v>51388.800000000003</v>
+      </c>
+      <c r="G106" s="121">
+        <f>F106*(1+'Demanda Dinamica'!$D$7)</f>
+        <v>54729.072</v>
+      </c>
+    </row>
+    <row r="107" spans="2:7">
+      <c r="B107" s="104" t="s">
+        <v>228</v>
+      </c>
+      <c r="C107" s="104"/>
+      <c r="D107" s="121">
+        <f>D55</f>
+        <v>0</v>
+      </c>
+      <c r="E107" s="121">
+        <f t="shared" ref="E107:G107" si="11">E55</f>
+        <v>0</v>
+      </c>
+      <c r="F107" s="121">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="G107" s="121">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:7">
+      <c r="B108" s="104" t="s">
+        <v>229</v>
+      </c>
+      <c r="C108" s="104"/>
+      <c r="D108" s="121">
+        <f>D56</f>
+        <v>10000</v>
+      </c>
+      <c r="E108" s="121">
+        <f t="shared" ref="E108:G108" si="12">E56</f>
+        <v>120000</v>
+      </c>
+      <c r="F108" s="121">
+        <f t="shared" si="12"/>
+        <v>127200</v>
+      </c>
+      <c r="G108" s="121">
+        <f t="shared" si="12"/>
+        <v>135468</v>
+      </c>
+    </row>
+    <row r="109" spans="2:7">
+      <c r="B109" s="104" t="s">
+        <v>230</v>
+      </c>
+      <c r="C109" s="104"/>
+      <c r="D109" s="121">
+        <f>D57</f>
+        <v>0</v>
+      </c>
+      <c r="E109" s="121">
+        <f t="shared" ref="E109:G109" si="13">E57</f>
+        <v>0</v>
+      </c>
+      <c r="F109" s="121">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="G109" s="121">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:7">
+      <c r="B110" s="104" t="s">
+        <v>231</v>
+      </c>
+      <c r="C110" s="104"/>
+      <c r="D110" s="121"/>
+      <c r="E110" s="121">
+        <f>G31</f>
+        <v>200000</v>
+      </c>
+      <c r="F110" s="121">
+        <f t="shared" ref="F110:G110" si="14">H31</f>
+        <v>200000</v>
+      </c>
+      <c r="G110" s="121">
+        <f t="shared" si="14"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
+      <c r="B111" s="104" t="s">
+        <v>232</v>
+      </c>
+      <c r="C111" s="104"/>
+      <c r="D111" s="121"/>
+      <c r="E111" s="121">
+        <f>G31</f>
+        <v>200000</v>
+      </c>
+      <c r="F111" s="121">
+        <f t="shared" ref="F111:G111" si="15">H31</f>
+        <v>200000</v>
+      </c>
+      <c r="G111" s="121">
+        <f t="shared" si="15"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7">
+      <c r="B112" s="104" t="s">
+        <v>233</v>
+      </c>
+      <c r="C112" s="104"/>
+      <c r="D112" s="121"/>
+      <c r="E112" s="121">
+        <f>E16/3</f>
+        <v>1616000</v>
+      </c>
+      <c r="F112" s="121">
+        <f>E112</f>
+        <v>1616000</v>
+      </c>
+      <c r="G112" s="121">
+        <f>F112</f>
+        <v>1616000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12">
+      <c r="B113" s="104" t="s">
+        <v>234</v>
+      </c>
+      <c r="C113" s="104"/>
+      <c r="D113" s="121"/>
+      <c r="E113" s="121">
+        <v>0</v>
+      </c>
+      <c r="F113" s="121">
+        <v>80000</v>
+      </c>
+      <c r="G113" s="121">
+        <f>F113+(F113*'Demanda Dinamica'!D7)</f>
+        <v>85200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12">
+      <c r="B114" s="104" t="s">
+        <v>235</v>
+      </c>
+      <c r="C114" s="104"/>
+      <c r="D114" s="121"/>
+      <c r="E114" s="121">
+        <v>0</v>
+      </c>
+      <c r="F114" s="121">
+        <v>0</v>
+      </c>
+      <c r="G114" s="121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12">
+      <c r="B115" s="96" t="s">
+        <v>237</v>
+      </c>
+      <c r="C115" s="97"/>
+      <c r="D115" s="98"/>
+      <c r="E115" s="125">
+        <f>SUM(E105:E114)</f>
+        <v>18446510</v>
+      </c>
+      <c r="F115" s="125">
+        <f t="shared" ref="F115:G115" si="16">SUM(F105:F114)</f>
+        <v>19512340.600000001</v>
+      </c>
+      <c r="G115" s="125">
+        <f t="shared" si="16"/>
+        <v>20649602.739000004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12">
+      <c r="B117" s="127" t="s">
+        <v>238</v>
+      </c>
+      <c r="C117" s="127"/>
+      <c r="D117" s="127"/>
+      <c r="E117" s="127"/>
+    </row>
+    <row r="118" spans="1:12">
+      <c r="A118" s="126"/>
+      <c r="B118" s="128" t="s">
+        <v>68</v>
+      </c>
+      <c r="C118" s="128" t="s">
+        <v>241</v>
+      </c>
+      <c r="D118" s="128" t="s">
+        <v>242</v>
+      </c>
+      <c r="E118" s="128" t="s">
+        <v>243</v>
+      </c>
+      <c r="F118" s="126"/>
+    </row>
+    <row r="119" spans="1:12">
+      <c r="B119" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C119" s="120">
+        <f>E115</f>
+        <v>18446510</v>
+      </c>
+      <c r="D119" s="120">
+        <f t="shared" ref="D119:E119" si="17">F115</f>
+        <v>19512340.600000001</v>
+      </c>
+      <c r="E119" s="120">
+        <f t="shared" si="17"/>
+        <v>20649602.739000004</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12">
+      <c r="B120" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C120" s="19">
+        <f>E75</f>
+        <v>45534530</v>
+      </c>
+      <c r="D120" s="19">
+        <f t="shared" ref="D120:E120" si="18">F75</f>
+        <v>48266601.799999997</v>
+      </c>
+      <c r="E120" s="19">
+        <f t="shared" si="18"/>
+        <v>48494274.450000003</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12">
+      <c r="B121" s="129" t="s">
+        <v>244</v>
+      </c>
+      <c r="C121" s="130">
+        <f>SUM(C119:C120)</f>
+        <v>63981040</v>
+      </c>
+      <c r="D121" s="130">
+        <f t="shared" ref="D121:E121" si="19">SUM(D119:D120)</f>
+        <v>67778942.400000006</v>
+      </c>
+      <c r="E121" s="130">
+        <f t="shared" si="19"/>
+        <v>69143877.18900001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12">
+      <c r="B123" s="131"/>
+      <c r="C123" s="132" t="s">
+        <v>245</v>
+      </c>
+      <c r="D123" s="132" t="s">
+        <v>246</v>
+      </c>
+      <c r="E123" s="132" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12">
+      <c r="B124" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="C124" s="120">
+        <f ca="1">C121/'Demanda Dinamica'!O13</f>
+        <v>298976.82242990652</v>
+      </c>
+      <c r="D124" s="120">
+        <f ca="1">D121/'Demanda Dinamica'!P13</f>
+        <v>187753.30304709144</v>
+      </c>
+      <c r="E124" s="120">
+        <f ca="1">E121/'Demanda Dinamica'!Q13</f>
+        <v>161929.45477517566</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12">
+      <c r="B125" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C125" s="120">
+        <f ca="1">C124+(C124*1.25)</f>
+        <v>672697.85046728968</v>
+      </c>
+      <c r="D125" s="120">
+        <f t="shared" ref="D125:E125" ca="1" si="20">D124+(D124*1.25)</f>
+        <v>422444.93185595574</v>
+      </c>
+      <c r="E125" s="120">
+        <f t="shared" ca="1" si="20"/>
+        <v>364341.27324414521</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12">
+      <c r="B127" s="133" t="s">
+        <v>264</v>
+      </c>
+      <c r="C127" s="133"/>
+      <c r="D127" s="133"/>
+      <c r="E127" s="133"/>
+      <c r="F127" s="133"/>
+      <c r="G127" s="133"/>
+      <c r="H127" s="133"/>
+      <c r="I127" s="133"/>
+      <c r="J127" s="133"/>
+      <c r="K127" s="133"/>
+      <c r="L127" s="133"/>
+    </row>
+    <row r="128" spans="1:12">
+      <c r="B128" s="69" t="s">
+        <v>249</v>
+      </c>
+      <c r="C128" s="69"/>
+      <c r="D128" s="69" t="s">
+        <v>256</v>
+      </c>
+      <c r="E128" s="69" t="s">
+        <v>259</v>
+      </c>
+      <c r="F128" s="69"/>
+      <c r="G128" s="69"/>
+      <c r="H128" s="68" t="s">
+        <v>260</v>
+      </c>
+      <c r="I128" s="68" t="s">
+        <v>261</v>
+      </c>
+      <c r="J128" s="68" t="s">
+        <v>262</v>
+      </c>
+      <c r="K128" s="68" t="s">
+        <v>263</v>
+      </c>
+      <c r="L128" s="68"/>
+    </row>
+    <row r="129" spans="2:20">
+      <c r="B129" s="69"/>
+      <c r="C129" s="69"/>
+      <c r="D129" s="69"/>
+      <c r="E129" s="61" t="s">
+        <v>125</v>
+      </c>
+      <c r="F129" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="G129" s="61" t="s">
+        <v>258</v>
+      </c>
+      <c r="H129" s="68"/>
+      <c r="I129" s="68"/>
+      <c r="J129" s="68"/>
+      <c r="K129" s="68"/>
+      <c r="L129" s="68"/>
+    </row>
+    <row r="130" spans="2:20">
+      <c r="B130" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D130" s="4">
+        <v>0</v>
+      </c>
+      <c r="E130" s="2">
+        <v>0</v>
+      </c>
+      <c r="F130" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="G130" s="2">
+        <v>0</v>
+      </c>
+      <c r="H130" s="2">
+        <v>0</v>
+      </c>
+      <c r="I130" s="2">
+        <v>0</v>
+      </c>
+      <c r="J130" s="2">
+        <v>0</v>
+      </c>
+      <c r="K130" s="2"/>
+      <c r="L130" s="2"/>
+    </row>
+    <row r="131" spans="2:20">
+      <c r="B131" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="D131" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E131" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F131" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="G131" s="2">
+        <f ca="1">'Demanda Dinamica'!$O$13/2</f>
+        <v>107</v>
+      </c>
+      <c r="H131" s="120">
+        <f ca="1">C125-(C125/4)</f>
+        <v>504523.38785046723</v>
+      </c>
+      <c r="I131" s="120">
+        <f ca="1">D125-(D125/4)</f>
+        <v>316833.69889196684</v>
+      </c>
+      <c r="J131" s="120">
+        <f ca="1">E125-(E125/4)</f>
+        <v>273255.95493310888</v>
+      </c>
+      <c r="K131" s="2"/>
+      <c r="L131" s="2"/>
+    </row>
+    <row r="132" spans="2:20">
+      <c r="B132" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D132" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="E132" s="2">
+        <v>3000</v>
+      </c>
+      <c r="F132" s="61" t="s">
+        <v>257</v>
+      </c>
+      <c r="G132" s="2">
+        <f ca="1">'Demanda Dinamica'!$O$13/2</f>
+        <v>107</v>
+      </c>
+      <c r="H132" s="120">
+        <f ca="1">C125</f>
+        <v>672697.85046728968</v>
+      </c>
+      <c r="I132" s="120">
+        <f ca="1">D125</f>
+        <v>422444.93185595574</v>
+      </c>
+      <c r="J132" s="120">
+        <f ca="1">E125</f>
+        <v>364341.27324414521</v>
+      </c>
+      <c r="K132" s="2"/>
+      <c r="L132" s="2"/>
+    </row>
+    <row r="133" spans="2:20">
+      <c r="D133" s="134">
+        <f>SUM(D130:D132)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="2:20">
+      <c r="B135" s="133" t="s">
+        <v>282</v>
+      </c>
+      <c r="C135" s="133"/>
+      <c r="D135" s="133"/>
+      <c r="E135" s="133"/>
+      <c r="F135" s="133"/>
+      <c r="G135" s="133"/>
+      <c r="H135" s="133"/>
+      <c r="I135" s="133"/>
+      <c r="J135" s="133"/>
+      <c r="K135" s="133"/>
+      <c r="L135" s="133"/>
+      <c r="M135" s="133"/>
+      <c r="N135" s="133"/>
+      <c r="O135" s="133"/>
+      <c r="P135" s="133"/>
+      <c r="Q135" s="133"/>
+    </row>
+    <row r="136" spans="2:20">
+      <c r="B136" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="F136" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G136" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H136" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="J136" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K136" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L136" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M136" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N136" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="O136" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="P136" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q136" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="137" spans="2:20">
+      <c r="B137" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!C13/2)</f>
+        <v>3531663.7149532707</v>
+      </c>
+      <c r="D137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!D13/2)</f>
+        <v>6054280.6542056073</v>
+      </c>
+      <c r="E137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!E13/2)</f>
+        <v>5297495.5724299056</v>
+      </c>
+      <c r="F137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!F13/2)</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="G137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!G13/2)</f>
+        <v>10594991.144859811</v>
+      </c>
+      <c r="H137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!H13/2)</f>
+        <v>2522616.939252336</v>
+      </c>
+      <c r="I137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!I13/2)</f>
+        <v>3027140.3271028036</v>
+      </c>
+      <c r="J137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!J13/2)</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="K137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!K13/2)</f>
+        <v>12613084.696261682</v>
+      </c>
+      <c r="L137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!L13/2)</f>
+        <v>10090467.757009344</v>
+      </c>
+      <c r="M137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!M13/2)</f>
+        <v>7567850.8177570086</v>
+      </c>
+      <c r="N137" s="137">
+        <f ca="1">$H$131*('Demanda Dinamica'!N13/2)</f>
+        <v>5802018.9602803728</v>
+      </c>
+      <c r="O137" s="137">
+        <f ca="1">SUM(C137:N137)</f>
+        <v>90309686.425233647</v>
+      </c>
+      <c r="P137" s="137">
+        <f ca="1">O137+(O137*'Demanda Dinamica'!$S$6)</f>
+        <v>97534461.339252338</v>
+      </c>
+      <c r="Q137" s="137">
+        <f ca="1">P137+(P137*'Demanda Dinamica'!$S$7)</f>
+        <v>112164630.54014018</v>
+      </c>
+    </row>
+    <row r="138" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B138" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!C13/2)</f>
+        <v>4708884.9532710277</v>
+      </c>
+      <c r="D138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!D13/2)</f>
+        <v>8072374.2056074757</v>
+      </c>
+      <c r="E138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!E13/2)</f>
+        <v>7063327.4299065415</v>
+      </c>
+      <c r="F138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!F13/2)</f>
+        <v>15472050.560747663</v>
+      </c>
+      <c r="G138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!G13/2)</f>
+        <v>14126654.859813083</v>
+      </c>
+      <c r="H138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!H13/2)</f>
+        <v>3363489.2523364485</v>
+      </c>
+      <c r="I138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!I13/2)</f>
+        <v>4036187.1028037379</v>
+      </c>
+      <c r="J138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!J13/2)</f>
+        <v>15472050.560747663</v>
+      </c>
+      <c r="K138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!K13/2)</f>
+        <v>16817446.261682242</v>
+      </c>
+      <c r="L138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!L13/2)</f>
+        <v>13453957.009345794</v>
+      </c>
+      <c r="M138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!M13/2)</f>
+        <v>10090467.757009346</v>
+      </c>
+      <c r="N138" s="137">
+        <f ca="1">$H$132*('Demanda Dinamica'!N13/2)</f>
+        <v>7736025.2803738313</v>
+      </c>
+      <c r="O138" s="137">
+        <f ca="1">SUM(C138:N138)</f>
+        <v>120412915.23364484</v>
+      </c>
+      <c r="P138" s="137">
+        <f ca="1">O138+(O138*'Demanda Dinamica'!$S$6)</f>
+        <v>130045948.45233643</v>
+      </c>
+      <c r="Q138" s="137">
+        <f ca="1">P138+(P138*'Demanda Dinamica'!$S$7)</f>
+        <v>149552840.72018689</v>
+      </c>
+    </row>
+    <row r="139" spans="2:20" ht="15.75" thickBot="1">
+      <c r="B139" s="22" t="s">
+        <v>274</v>
+      </c>
+      <c r="C139" s="138">
+        <f ca="1">SUM(C137:C138)</f>
+        <v>8240548.6682242984</v>
+      </c>
+      <c r="D139" s="138">
+        <f t="shared" ref="D139:L139" ca="1" si="21">SUM(D137:D138)</f>
+        <v>14126654.859813083</v>
+      </c>
+      <c r="E139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>12360823.002336446</v>
+      </c>
+      <c r="F139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>27076088.481308408</v>
+      </c>
+      <c r="G139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>24721646.004672892</v>
+      </c>
+      <c r="H139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>5886106.1915887846</v>
+      </c>
+      <c r="I139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>7063327.4299065415</v>
+      </c>
+      <c r="J139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>27076088.481308408</v>
+      </c>
+      <c r="K139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>29430530.957943924</v>
+      </c>
+      <c r="L139" s="138">
+        <f t="shared" ca="1" si="21"/>
+        <v>23544424.766355138</v>
+      </c>
+      <c r="M139" s="138">
+        <f t="shared" ref="M139" ca="1" si="22">SUM(M137:M138)</f>
+        <v>17658318.574766353</v>
+      </c>
+      <c r="N139" s="138">
+        <f t="shared" ref="N139" ca="1" si="23">SUM(N137:N138)</f>
+        <v>13538044.240654204</v>
+      </c>
+      <c r="O139" s="138">
+        <f ca="1">SUM(C139:N139)</f>
+        <v>210722601.65887848</v>
+      </c>
+      <c r="P139" s="138">
+        <f ca="1">O139+(O139*'Demanda Dinamica'!$S$6)</f>
+        <v>227580409.79158875</v>
+      </c>
+      <c r="Q139" s="138">
+        <f ca="1">P139+(P139*'Demanda Dinamica'!$S$7)</f>
+        <v>261717471.26032707</v>
+      </c>
+      <c r="S139" s="135" t="s">
+        <v>271</v>
+      </c>
+      <c r="T139" s="136">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="140" spans="2:20">
+      <c r="B140" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C140" s="137">
+        <f ca="1">C139*0.19</f>
+        <v>1565704.2469626167</v>
+      </c>
+      <c r="D140" s="137">
+        <f t="shared" ref="D140:P140" ca="1" si="24">D139*0.19</f>
+        <v>2684064.4233644856</v>
+      </c>
+      <c r="E140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>2348556.3704439248</v>
+      </c>
+      <c r="F140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>5144456.8114485973</v>
+      </c>
+      <c r="G140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>4697112.7408878496</v>
+      </c>
+      <c r="H140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>1118360.1764018692</v>
+      </c>
+      <c r="I140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>1342032.2116822428</v>
+      </c>
+      <c r="J140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>5144456.8114485973</v>
+      </c>
+      <c r="K140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>5591800.882009346</v>
+      </c>
+      <c r="L140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>4473440.7056074766</v>
+      </c>
+      <c r="M140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>3355080.5292056073</v>
+      </c>
+      <c r="N140" s="137">
+        <f t="shared" ca="1" si="24"/>
+        <v>2572228.4057242987</v>
+      </c>
+      <c r="O140" s="137">
+        <f ca="1">SUM(C140:N140)</f>
+        <v>40037294.31518691</v>
+      </c>
+      <c r="P140" s="137">
+        <f ca="1">O140+(O140*'Demanda Dinamica'!$S$6)</f>
+        <v>43240277.860401861</v>
+      </c>
+      <c r="Q140" s="137">
+        <f ca="1">P140+(P140*'Demanda Dinamica'!$S$7)</f>
+        <v>49726319.539462142</v>
+      </c>
+    </row>
+    <row r="141" spans="2:20">
+      <c r="B141" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C141" s="137">
+        <f ca="1">C140*0.15</f>
+        <v>234855.6370443925</v>
+      </c>
+      <c r="D141" s="137">
+        <f t="shared" ref="D141:J141" ca="1" si="25">D140*0.15</f>
+        <v>402609.66350467282</v>
+      </c>
+      <c r="E141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>352283.45556658873</v>
+      </c>
+      <c r="F141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>771668.52171728958</v>
+      </c>
+      <c r="G141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>704566.91113317746</v>
+      </c>
+      <c r="H141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>167754.02646028038</v>
+      </c>
+      <c r="I141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>201304.83175233641</v>
+      </c>
+      <c r="J141" s="137">
+        <f t="shared" ca="1" si="25"/>
+        <v>771668.52171728958</v>
+      </c>
+      <c r="K141" s="137">
+        <f t="shared" ref="K141" ca="1" si="26">K140*0.15</f>
+        <v>838770.13230140193</v>
+      </c>
+      <c r="L141" s="137">
+        <f t="shared" ref="L141" ca="1" si="27">L140*0.15</f>
+        <v>671016.10584112152</v>
+      </c>
+      <c r="M141" s="137">
+        <f t="shared" ref="M141" ca="1" si="28">M140*0.15</f>
+        <v>503262.07938084105</v>
+      </c>
+      <c r="N141" s="137">
+        <f t="shared" ref="N141" ca="1" si="29">N140*0.15</f>
+        <v>385834.26085864479</v>
+      </c>
+      <c r="O141" s="137">
+        <f ca="1">SUM(C141:N141)</f>
+        <v>6005594.1472780369</v>
+      </c>
+      <c r="P141" s="137">
+        <f ca="1">O141+(O141*'Demanda Dinamica'!$S$6)</f>
+        <v>6486041.6790602803</v>
+      </c>
+      <c r="Q141" s="137">
+        <f ca="1">P141+(P141*'Demanda Dinamica'!$S$7)</f>
+        <v>7458947.9309193222</v>
+      </c>
+    </row>
+    <row r="142" spans="2:20">
+      <c r="B142" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C142" s="137">
+        <f ca="1">C139+C140-C141</f>
+        <v>9571397.278142523</v>
+      </c>
+      <c r="D142" s="137">
+        <f t="shared" ref="D142:N142" ca="1" si="30">D139+D140-D141</f>
+        <v>16408109.619672896</v>
+      </c>
+      <c r="E142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>14357095.917213783</v>
+      </c>
+      <c r="F142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>31448876.771039713</v>
+      </c>
+      <c r="G142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>28714191.834427565</v>
+      </c>
+      <c r="H142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>6836712.3415303733</v>
+      </c>
+      <c r="I142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>8204054.8098364482</v>
+      </c>
+      <c r="J142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>31448876.771039713</v>
+      </c>
+      <c r="K142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>34183561.707651868</v>
+      </c>
+      <c r="L142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>27346849.366121493</v>
+      </c>
+      <c r="M142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>20510137.024591118</v>
+      </c>
+      <c r="N142" s="137">
+        <f t="shared" ca="1" si="30"/>
+        <v>15724438.385519857</v>
+      </c>
+      <c r="O142" s="137">
+        <f ca="1">SUM(C142:N142)</f>
+        <v>244754301.82678735</v>
+      </c>
+      <c r="P142" s="137">
+        <f ca="1">O142+(O142*'Demanda Dinamica'!$S$6)</f>
+        <v>264334645.97293034</v>
+      </c>
+      <c r="Q142" s="137">
+        <f ca="1">P142+(P142*'Demanda Dinamica'!$S$7)</f>
+        <v>303984842.8688699</v>
+      </c>
+    </row>
+    <row r="143" spans="2:20">
+      <c r="B143" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C143" s="137">
+        <f ca="1">(C138+(C138*0.19))-(C138*0.19*0.15)</f>
+        <v>5469369.8732242985</v>
+      </c>
+      <c r="D143" s="137">
+        <f t="shared" ref="D143:N143" ca="1" si="31">(D138+(D138*0.19))-(D138*0.19*0.15)</f>
+        <v>9376062.6398130842</v>
+      </c>
+      <c r="E143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>8204054.8098364482</v>
+      </c>
+      <c r="F143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>17970786.726308409</v>
+      </c>
+      <c r="G143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>16408109.619672896</v>
+      </c>
+      <c r="H143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>3906692.7665887848</v>
+      </c>
+      <c r="I143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>4688031.3199065421</v>
+      </c>
+      <c r="J143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>17970786.726308409</v>
+      </c>
+      <c r="K143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>19533463.832943924</v>
+      </c>
+      <c r="L143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>15626771.066355139</v>
+      </c>
+      <c r="M143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>11720078.299766354</v>
+      </c>
+      <c r="N143" s="137">
+        <f t="shared" ca="1" si="31"/>
+        <v>8985393.3631542046</v>
+      </c>
+      <c r="O143" s="137">
+        <f ca="1">SUM(C143:N143)</f>
+        <v>139859601.0438785</v>
+      </c>
+      <c r="P143" s="137">
+        <f ca="1">O143+(O143*'Demanda Dinamica'!$S$6)</f>
+        <v>151048369.12738878</v>
+      </c>
+      <c r="Q143" s="137">
+        <f ca="1">P143+(P143*'Demanda Dinamica'!$S$7)</f>
+        <v>173705624.49649709</v>
+      </c>
+    </row>
+    <row r="144" spans="2:20">
+      <c r="B144" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C144" s="137">
+        <f ca="1">(C137+(C137*0.19))-(C137*0.19*0.15)</f>
+        <v>4102027.4049182241</v>
+      </c>
+      <c r="D144" s="137">
+        <f t="shared" ref="D144:N144" ca="1" si="32">(D137+(D137*0.19))-(D137*0.19*0.15)</f>
+        <v>7032046.9798598131</v>
+      </c>
+      <c r="E144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>6153041.1073773354</v>
+      </c>
+      <c r="F144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>13478090.044731306</v>
+      </c>
+      <c r="G144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>12306082.214754671</v>
+      </c>
+      <c r="H144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>2930019.5749415881</v>
+      </c>
+      <c r="I144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>3516023.4899299066</v>
+      </c>
+      <c r="J144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>13478090.044731306</v>
+      </c>
+      <c r="K144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>14650097.874707943</v>
+      </c>
+      <c r="L144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>11720078.299766352</v>
+      </c>
+      <c r="M144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>8790058.7248247657</v>
+      </c>
+      <c r="N144" s="137">
+        <f t="shared" ca="1" si="32"/>
+        <v>6739045.022365653</v>
+      </c>
+      <c r="O144" s="137">
+        <f ca="1">SUM(C144:N144)</f>
+        <v>104894700.78290887</v>
+      </c>
+      <c r="P144" s="137">
+        <f ca="1">O144+(O144*'Demanda Dinamica'!$S$6)</f>
+        <v>113286276.84554158</v>
+      </c>
+      <c r="Q144" s="137">
+        <f ca="1">P144+(P144*'Demanda Dinamica'!$S$7)</f>
+        <v>130279218.37237282</v>
+      </c>
+    </row>
+    <row r="145" spans="2:17">
+      <c r="B145" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!C13/2</f>
+        <v>3531663.7149532707</v>
+      </c>
+      <c r="D145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!D13/2</f>
+        <v>6054280.6542056073</v>
+      </c>
+      <c r="E145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!E13/2</f>
+        <v>5297495.5724299056</v>
+      </c>
+      <c r="F145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!F13/2</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="G145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!G13/2</f>
+        <v>10594991.144859811</v>
+      </c>
+      <c r="H145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!H13/2</f>
+        <v>2522616.939252336</v>
+      </c>
+      <c r="I145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!I13/2</f>
+        <v>3027140.3271028036</v>
+      </c>
+      <c r="J145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!J13/2</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="K145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!K13/2</f>
+        <v>12613084.696261682</v>
+      </c>
+      <c r="L145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!L13/2</f>
+        <v>10090467.757009344</v>
+      </c>
+      <c r="M145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!M13/2</f>
+        <v>7567850.8177570086</v>
+      </c>
+      <c r="N145" s="137">
+        <f ca="1">$H$131*'Demanda Dinamica'!N13/2</f>
+        <v>5802018.9602803728</v>
+      </c>
+      <c r="O145" s="137">
+        <f t="shared" ref="O145:O147" ca="1" si="33">SUM(C145:N145)</f>
+        <v>90309686.425233647</v>
+      </c>
+      <c r="P145" s="137">
+        <f ca="1">O145+(O145*'Demanda Dinamica'!$S$6)</f>
+        <v>97534461.339252338</v>
+      </c>
+      <c r="Q145" s="137">
+        <f ca="1">P145+(P145*'Demanda Dinamica'!$S$7)</f>
+        <v>112164630.54014018</v>
+      </c>
+    </row>
+    <row r="146" spans="2:17">
+      <c r="B146" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C146" s="137">
+        <f ca="1">C143+C144</f>
+        <v>9571397.278142523</v>
+      </c>
+      <c r="D146" s="137">
+        <f t="shared" ref="D146:M146" ca="1" si="34">D143+D144</f>
+        <v>16408109.619672898</v>
+      </c>
+      <c r="E146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>14357095.917213783</v>
+      </c>
+      <c r="F146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>31448876.771039717</v>
+      </c>
+      <c r="G146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>28714191.834427565</v>
+      </c>
+      <c r="H146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>6836712.3415303733</v>
+      </c>
+      <c r="I146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>8204054.8098364491</v>
+      </c>
+      <c r="J146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>31448876.771039717</v>
+      </c>
+      <c r="K146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>34183561.707651868</v>
+      </c>
+      <c r="L146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>27346849.366121493</v>
+      </c>
+      <c r="M146" s="137">
+        <f t="shared" ca="1" si="34"/>
+        <v>20510137.024591118</v>
+      </c>
+      <c r="N146" s="137">
+        <f ca="1">N143+N144</f>
+        <v>15724438.385519858</v>
+      </c>
+      <c r="O146" s="137">
+        <f t="shared" ca="1" si="33"/>
+        <v>244754301.82678735</v>
+      </c>
+      <c r="P146" s="137">
+        <f ca="1">O146+(O146*'Demanda Dinamica'!$S$6)</f>
+        <v>264334645.97293034</v>
+      </c>
+      <c r="Q146" s="137">
+        <f ca="1">P146+(P146*'Demanda Dinamica'!$S$7)</f>
+        <v>303984842.8688699</v>
+      </c>
+    </row>
+    <row r="147" spans="2:17">
+      <c r="B147" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!C13/2)</f>
+        <v>3531663.7149532707</v>
+      </c>
+      <c r="D147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!D13/2)</f>
+        <v>6054280.6542056073</v>
+      </c>
+      <c r="E147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!E13/2)</f>
+        <v>5297495.5724299056</v>
+      </c>
+      <c r="F147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!F13/2)</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="G147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!G13/2)</f>
+        <v>10594991.144859811</v>
+      </c>
+      <c r="H147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!H13/2)</f>
+        <v>2522616.939252336</v>
+      </c>
+      <c r="I147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!I13/2)</f>
+        <v>3027140.3271028036</v>
+      </c>
+      <c r="J147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!J13/2)</f>
+        <v>11604037.920560746</v>
+      </c>
+      <c r="K147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!K13/2)</f>
+        <v>12613084.696261682</v>
+      </c>
+      <c r="L147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!L13/2)</f>
+        <v>10090467.757009344</v>
+      </c>
+      <c r="M147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!M13/2)</f>
+        <v>7567850.8177570086</v>
+      </c>
+      <c r="N147" s="40">
+        <f ca="1">$H$131*('Demanda Dinamica'!N13/2)</f>
+        <v>5802018.9602803728</v>
+      </c>
+      <c r="O147" s="137">
+        <f t="shared" ca="1" si="33"/>
+        <v>90309686.425233647</v>
+      </c>
+      <c r="P147" s="137">
+        <f ca="1">O147+(O147*'Demanda Dinamica'!$S$6)</f>
+        <v>97534461.339252338</v>
+      </c>
+      <c r="Q147" s="137">
+        <f ca="1">P147+(P147*'Demanda Dinamica'!$S$7)</f>
+        <v>112164630.54014018</v>
+      </c>
+    </row>
+    <row r="149" spans="2:17">
+      <c r="B149" s="139" t="s">
+        <v>283</v>
+      </c>
+      <c r="C149" s="139"/>
+      <c r="D149" s="139"/>
+      <c r="E149" s="139"/>
+      <c r="G149" s="140" t="s">
+        <v>2</v>
+      </c>
+      <c r="H149" s="140"/>
+      <c r="I149" s="140"/>
+      <c r="J149" s="140"/>
+      <c r="K149" s="140"/>
+    </row>
+    <row r="150" spans="2:17">
+      <c r="B150" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C150" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D150" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="E150" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="G150" s="141" t="s">
+        <v>290</v>
+      </c>
+      <c r="H150" s="141" t="s">
+        <v>291</v>
+      </c>
+      <c r="I150" s="141" t="s">
+        <v>292</v>
+      </c>
+      <c r="J150" s="141" t="s">
+        <v>293</v>
+      </c>
+      <c r="K150" s="141" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="151" spans="2:17" ht="21" customHeight="1">
+      <c r="B151" s="59" t="s">
+        <v>284</v>
+      </c>
+      <c r="C151" s="144">
+        <f ca="1">0*'Demanda Dinamica'!O13</f>
+        <v>0</v>
+      </c>
+      <c r="D151" s="144">
+        <f ca="1">0*'Demanda Dinamica'!P13</f>
+        <v>0</v>
+      </c>
+      <c r="E151" s="144">
+        <f ca="1">0*'Demanda Dinamica'!Q13</f>
+        <v>0</v>
+      </c>
+      <c r="G151" s="142">
+        <f ca="1">O139</f>
+        <v>210722601.65887848</v>
+      </c>
+      <c r="H151" s="143">
+        <f ca="1">C124*'Demanda Dinamica'!O13</f>
+        <v>63981039.999999993</v>
+      </c>
+      <c r="I151" s="143">
+        <f ca="1">G151-H151-J151-K151</f>
+        <v>125669301.49299064</v>
+      </c>
+      <c r="J151" s="143">
+        <f ca="1">G151*0.05</f>
+        <v>10536130.082943924</v>
+      </c>
+      <c r="K151" s="143">
+        <f ca="1">J151</f>
+        <v>10536130.082943924</v>
+      </c>
+    </row>
+    <row r="152" spans="2:17" ht="30">
+      <c r="B152" s="59" t="s">
+        <v>285</v>
+      </c>
+      <c r="C152" s="144">
+        <f ca="1">O139*0.05</f>
+        <v>10536130.082943924</v>
+      </c>
+      <c r="D152" s="144">
+        <f t="shared" ref="D152:E152" ca="1" si="35">P139*0.05</f>
+        <v>11379020.489579439</v>
+      </c>
+      <c r="E152" s="144">
+        <f t="shared" ca="1" si="35"/>
+        <v>13085873.563016355</v>
+      </c>
+    </row>
+    <row r="153" spans="2:17" ht="30">
+      <c r="B153" s="59" t="s">
+        <v>286</v>
+      </c>
+      <c r="C153" s="144">
+        <f ca="1">C152</f>
+        <v>10536130.082943924</v>
+      </c>
+      <c r="D153" s="144">
+        <f t="shared" ref="D153:E153" ca="1" si="36">D152</f>
+        <v>11379020.489579439</v>
+      </c>
+      <c r="E153" s="144">
+        <f t="shared" ca="1" si="36"/>
+        <v>13085873.563016355</v>
+      </c>
+    </row>
+    <row r="154" spans="2:17" ht="30">
+      <c r="B154" s="59" t="s">
+        <v>287</v>
+      </c>
+      <c r="C154" s="144">
+        <f ca="1">(G151/1000)*11</f>
+        <v>2317948.6182476631</v>
+      </c>
+      <c r="D154" s="144">
+        <f ca="1">C154+(C154*'Demanda Dinamica'!$D$6)</f>
+        <v>2457025.5353425229</v>
+      </c>
+      <c r="E154" s="144">
+        <f ca="1">D154+('Demanda Dinamica'!$D$7*D154)</f>
+        <v>2616732.1951397867</v>
+      </c>
+    </row>
+    <row r="155" spans="2:17" ht="30">
+      <c r="B155" s="59" t="s">
+        <v>288</v>
+      </c>
+      <c r="C155" s="144">
+        <f ca="1">C154*0.15</f>
+        <v>347692.29273714946</v>
+      </c>
+      <c r="D155" s="144">
+        <f t="shared" ref="D155:E155" ca="1" si="37">D154*0.15</f>
+        <v>368553.83030137845</v>
+      </c>
+      <c r="E155" s="144">
+        <f t="shared" ca="1" si="37"/>
+        <v>392509.82927096798</v>
+      </c>
+    </row>
+    <row r="156" spans="2:17">
+      <c r="B156" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="C156" s="145">
+        <f ca="1">SUM(C151:C155)</f>
+        <v>23737901.076872658</v>
+      </c>
+      <c r="D156" s="145">
+        <f t="shared" ref="D156:E156" ca="1" si="38">SUM(D151:D155)</f>
+        <v>25583620.344802778</v>
+      </c>
+      <c r="E156" s="145">
+        <f t="shared" ca="1" si="38"/>
+        <v>29180989.150443465</v>
+      </c>
+    </row>
+    <row r="158" spans="2:17">
+      <c r="B158" s="89" t="s">
+        <v>318</v>
+      </c>
+      <c r="C158" s="89"/>
+      <c r="D158" s="89"/>
+      <c r="E158" s="89"/>
+      <c r="F158" s="89"/>
+      <c r="G158" s="89"/>
+    </row>
+    <row r="159" spans="2:17">
+      <c r="B159" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="C159" s="88"/>
+      <c r="D159" s="88"/>
+      <c r="E159" s="62" t="s">
+        <v>2</v>
+      </c>
+      <c r="F159" s="62" t="s">
+        <v>3</v>
+      </c>
+      <c r="G159" s="62" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="160" spans="2:17">
+      <c r="B160" s="71" t="s">
+        <v>295</v>
+      </c>
+      <c r="C160" s="69" t="s">
+        <v>296</v>
+      </c>
+      <c r="D160" s="69"/>
+      <c r="E160" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F160" s="137">
+        <f>F113</f>
+        <v>80000</v>
+      </c>
+      <c r="G160" s="137">
+        <f>G113</f>
+        <v>85200</v>
+      </c>
+    </row>
+    <row r="161" spans="2:7">
+      <c r="B161" s="71"/>
+      <c r="C161" s="69" t="s">
+        <v>298</v>
+      </c>
+      <c r="D161" s="69"/>
+      <c r="E161" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F161" s="137">
+        <v>0</v>
+      </c>
+      <c r="G161" s="137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="2:7">
+      <c r="B162" s="71"/>
+      <c r="C162" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="D162" s="79"/>
+      <c r="E162" s="120">
+        <f>'Demanda Dinamica'!V43</f>
+        <v>45334530</v>
+      </c>
+      <c r="F162" s="120">
+        <f>'Demanda Dinamica'!W43</f>
+        <v>48054601.800000004</v>
+      </c>
+      <c r="G162" s="120">
+        <f>'Demanda Dinamica'!X43</f>
+        <v>51178150.917000011</v>
+      </c>
+    </row>
+    <row r="163" spans="2:7">
+      <c r="B163" s="71"/>
+      <c r="C163" s="69" t="s">
+        <v>300</v>
+      </c>
+      <c r="D163" s="69"/>
+      <c r="E163" s="120">
+        <f>'Demanda Dinamica'!V35</f>
+        <v>2400000</v>
+      </c>
+      <c r="F163" s="120">
+        <f>'Demanda Dinamica'!W35</f>
+        <v>2544000</v>
+      </c>
+      <c r="G163" s="120">
+        <f>'Demanda Dinamica'!X35</f>
+        <v>2709360</v>
+      </c>
+    </row>
+    <row r="164" spans="2:7">
+      <c r="B164" s="71"/>
+      <c r="C164" s="69" t="s">
+        <v>301</v>
+      </c>
+      <c r="D164" s="69"/>
+      <c r="E164" s="120">
+        <v>0</v>
+      </c>
+      <c r="F164" s="137">
+        <v>0</v>
+      </c>
+      <c r="G164" s="137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="2:7">
+      <c r="B165" s="71"/>
+      <c r="C165" s="69" t="s">
+        <v>302</v>
+      </c>
+      <c r="D165" s="69"/>
+      <c r="E165" s="120">
+        <f>E106</f>
+        <v>48480</v>
+      </c>
+      <c r="F165" s="120">
+        <f t="shared" ref="F165:G165" si="39">F106</f>
+        <v>51388.800000000003</v>
+      </c>
+      <c r="G165" s="120">
+        <f t="shared" si="39"/>
+        <v>54729.072</v>
+      </c>
+    </row>
+    <row r="166" spans="2:7">
+      <c r="B166" s="71"/>
+      <c r="C166" s="69" t="s">
+        <v>303</v>
+      </c>
+      <c r="D166" s="69"/>
+      <c r="E166" s="120">
+        <f>E107</f>
+        <v>0</v>
+      </c>
+      <c r="F166" s="120">
+        <f t="shared" ref="F166:G166" si="40">F107</f>
+        <v>0</v>
+      </c>
+      <c r="G166" s="120">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="2:7">
+      <c r="B167" s="71"/>
+      <c r="C167" s="69" t="s">
+        <v>304</v>
+      </c>
+      <c r="D167" s="69"/>
+      <c r="E167" s="120">
+        <f t="shared" ref="E167:G169" si="41">E108</f>
+        <v>120000</v>
+      </c>
+      <c r="F167" s="120">
+        <f t="shared" si="41"/>
+        <v>127200</v>
+      </c>
+      <c r="G167" s="120">
+        <f t="shared" si="41"/>
+        <v>135468</v>
+      </c>
+    </row>
+    <row r="168" spans="2:7">
+      <c r="B168" s="71"/>
+      <c r="C168" s="69" t="s">
+        <v>305</v>
+      </c>
+      <c r="D168" s="69"/>
+      <c r="E168" s="120">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="F168" s="120">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="G168" s="120">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="2:7">
+      <c r="B169" s="71"/>
+      <c r="C169" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="D169" s="69"/>
+      <c r="E169" s="120">
+        <f>E110</f>
+        <v>200000</v>
+      </c>
+      <c r="F169" s="120">
+        <f t="shared" ref="F169:G169" si="42">F110</f>
+        <v>200000</v>
+      </c>
+      <c r="G169" s="120">
+        <f t="shared" si="42"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="170" spans="2:7">
+      <c r="B170" s="71"/>
+      <c r="C170" s="69" t="s">
+        <v>306</v>
+      </c>
+      <c r="D170" s="69"/>
+      <c r="E170" s="120">
+        <f>E111</f>
+        <v>200000</v>
+      </c>
+      <c r="F170" s="120">
+        <f t="shared" ref="F170:G170" si="43">F111</f>
+        <v>200000</v>
+      </c>
+      <c r="G170" s="120">
+        <f t="shared" si="43"/>
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="171" spans="2:7">
+      <c r="B171" s="71"/>
+      <c r="C171" s="69" t="s">
+        <v>319</v>
+      </c>
+      <c r="D171" s="69"/>
+      <c r="E171" s="120">
+        <v>0</v>
+      </c>
+      <c r="F171" s="137">
+        <v>0</v>
+      </c>
+      <c r="G171" s="137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="2:7">
+      <c r="B172" s="71"/>
+      <c r="C172" s="88" t="s">
+        <v>307</v>
+      </c>
+      <c r="D172" s="88"/>
+      <c r="E172" s="124">
+        <f>SUM(E162:E171)</f>
+        <v>48303010</v>
+      </c>
+      <c r="F172" s="138">
+        <f>SUM(F160:F171)</f>
+        <v>51257190.600000001</v>
+      </c>
+      <c r="G172" s="138">
+        <f>SUM(G160:G171)</f>
+        <v>54562907.989000008</v>
+      </c>
+    </row>
+    <row r="173" spans="2:7">
+      <c r="B173" s="88" t="s">
+        <v>308</v>
+      </c>
+      <c r="C173" s="69" t="s">
+        <v>186</v>
+      </c>
+      <c r="D173" s="69"/>
+      <c r="E173" s="120">
+        <f>E64</f>
+        <v>0</v>
+      </c>
+      <c r="F173" s="120">
+        <f t="shared" ref="F173:G173" si="44">F64</f>
+        <v>0</v>
+      </c>
+      <c r="G173" s="120">
+        <f t="shared" si="44"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="2:7">
+      <c r="B174" s="88"/>
+      <c r="C174" s="69" t="s">
+        <v>309</v>
+      </c>
+      <c r="D174" s="69"/>
+      <c r="E174" s="120">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="F174" s="120">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G174" s="120">
+        <f>0</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="2:7">
+      <c r="B175" s="88"/>
+      <c r="C175" s="69" t="s">
+        <v>310</v>
+      </c>
+      <c r="D175" s="69"/>
+      <c r="E175" s="120">
+        <v>0</v>
+      </c>
+      <c r="F175" s="120">
+        <v>0</v>
+      </c>
+      <c r="G175" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="2:7">
+      <c r="B176" s="88"/>
+      <c r="C176" s="69" t="s">
+        <v>311</v>
+      </c>
+      <c r="D176" s="69"/>
+      <c r="E176" s="120">
+        <v>0</v>
+      </c>
+      <c r="F176" s="120">
+        <v>0</v>
+      </c>
+      <c r="G176" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="2:7">
+      <c r="B177" s="88"/>
+      <c r="C177" s="69" t="s">
+        <v>284</v>
+      </c>
+      <c r="D177" s="69"/>
+      <c r="E177" s="120">
+        <v>0</v>
+      </c>
+      <c r="F177" s="120">
+        <v>0</v>
+      </c>
+      <c r="G177" s="120">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="2:7">
+      <c r="B178" s="88"/>
+      <c r="C178" s="69" t="s">
+        <v>312</v>
+      </c>
+      <c r="D178" s="69"/>
+      <c r="E178" s="120">
+        <f ca="1">C152</f>
+        <v>10536130.082943924</v>
+      </c>
+      <c r="F178" s="120">
+        <f t="shared" ref="F178:G178" ca="1" si="45">D152</f>
+        <v>11379020.489579439</v>
+      </c>
+      <c r="G178" s="120">
+        <f t="shared" ca="1" si="45"/>
+        <v>13085873.563016355</v>
+      </c>
+    </row>
+    <row r="179" spans="2:7">
+      <c r="B179" s="88"/>
+      <c r="C179" s="69" t="s">
+        <v>313</v>
+      </c>
+      <c r="D179" s="69"/>
+      <c r="E179" s="120">
+        <f ca="1">C153</f>
+        <v>10536130.082943924</v>
+      </c>
+      <c r="F179" s="120">
+        <f t="shared" ref="F179:G181" ca="1" si="46">D153</f>
+        <v>11379020.489579439</v>
+      </c>
+      <c r="G179" s="120">
+        <f t="shared" ca="1" si="46"/>
+        <v>13085873.563016355</v>
+      </c>
+    </row>
+    <row r="180" spans="2:7">
+      <c r="B180" s="88"/>
+      <c r="C180" s="69" t="s">
+        <v>314</v>
+      </c>
+      <c r="D180" s="69"/>
+      <c r="E180" s="120">
+        <f t="shared" ref="E180:E181" ca="1" si="47">C154</f>
+        <v>2317948.6182476631</v>
+      </c>
+      <c r="F180" s="120">
+        <f t="shared" ca="1" si="46"/>
+        <v>2457025.5353425229</v>
+      </c>
+      <c r="G180" s="120">
+        <f t="shared" ca="1" si="46"/>
+        <v>2616732.1951397867</v>
+      </c>
+    </row>
+    <row r="181" spans="2:7">
+      <c r="B181" s="88"/>
+      <c r="C181" s="69" t="s">
+        <v>315</v>
+      </c>
+      <c r="D181" s="69"/>
+      <c r="E181" s="120">
+        <f t="shared" ca="1" si="47"/>
+        <v>347692.29273714946</v>
+      </c>
+      <c r="F181" s="120">
+        <f t="shared" ca="1" si="46"/>
+        <v>368553.83030137845</v>
+      </c>
+      <c r="G181" s="120">
+        <f t="shared" ca="1" si="46"/>
+        <v>392509.82927096798</v>
+      </c>
+    </row>
+    <row r="182" spans="2:7">
+      <c r="B182" s="88"/>
+      <c r="C182" s="88" t="s">
+        <v>316</v>
+      </c>
+      <c r="D182" s="88"/>
+      <c r="E182" s="124">
+        <f ca="1">SUM(E173:E181)</f>
+        <v>23737901.076872658</v>
+      </c>
+      <c r="F182" s="124">
+        <f t="shared" ref="F182:G182" ca="1" si="48">SUM(F173:F181)</f>
+        <v>25583620.344802778</v>
+      </c>
+      <c r="G182" s="124">
+        <f t="shared" ca="1" si="48"/>
+        <v>29180989.150443465</v>
+      </c>
+    </row>
+    <row r="183" spans="2:7">
+      <c r="B183" s="146" t="s">
+        <v>317</v>
+      </c>
+      <c r="C183" s="146"/>
+      <c r="D183" s="146"/>
+      <c r="E183" s="147">
+        <f ca="1">E172+E182</f>
+        <v>72040911.076872662</v>
+      </c>
+      <c r="F183" s="147">
+        <f t="shared" ref="F183:G183" ca="1" si="49">F172+F182</f>
+        <v>76840810.944802776</v>
+      </c>
+      <c r="G183" s="147">
+        <f t="shared" ca="1" si="49"/>
+        <v>83743897.139443472</v>
+      </c>
+    </row>
+    <row r="185" spans="2:7">
+      <c r="B185" s="148" t="s">
+        <v>321</v>
+      </c>
+      <c r="C185" s="148"/>
+      <c r="D185" s="148"/>
+      <c r="E185" s="148"/>
+      <c r="F185" s="148"/>
+    </row>
+    <row r="186" spans="2:7">
+      <c r="B186" t="s">
+        <v>68</v>
+      </c>
+      <c r="C186" t="s">
+        <v>320</v>
+      </c>
+      <c r="D186" t="s">
+        <v>2</v>
+      </c>
+      <c r="E186" t="s">
+        <v>3</v>
+      </c>
+      <c r="F186" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="64">
+  <mergeCells count="118">
+    <mergeCell ref="B183:D183"/>
+    <mergeCell ref="B185:F185"/>
+    <mergeCell ref="C171:D171"/>
+    <mergeCell ref="C172:D172"/>
+    <mergeCell ref="B173:B182"/>
+    <mergeCell ref="C173:D173"/>
+    <mergeCell ref="C174:D174"/>
+    <mergeCell ref="C175:D175"/>
+    <mergeCell ref="C176:D176"/>
+    <mergeCell ref="C177:D177"/>
+    <mergeCell ref="C178:D178"/>
+    <mergeCell ref="C179:D179"/>
+    <mergeCell ref="C180:D180"/>
+    <mergeCell ref="C181:D181"/>
+    <mergeCell ref="C182:D182"/>
+    <mergeCell ref="B149:E149"/>
+    <mergeCell ref="G149:K149"/>
+    <mergeCell ref="B158:G158"/>
+    <mergeCell ref="B159:D159"/>
+    <mergeCell ref="B160:B172"/>
+    <mergeCell ref="C160:D160"/>
+    <mergeCell ref="C161:D161"/>
+    <mergeCell ref="C162:D162"/>
+    <mergeCell ref="C163:D163"/>
+    <mergeCell ref="C164:D164"/>
+    <mergeCell ref="C165:D165"/>
+    <mergeCell ref="C166:D166"/>
+    <mergeCell ref="C167:D167"/>
+    <mergeCell ref="C168:D168"/>
+    <mergeCell ref="C169:D169"/>
+    <mergeCell ref="C170:D170"/>
+    <mergeCell ref="I128:I129"/>
+    <mergeCell ref="J128:J129"/>
+    <mergeCell ref="K128:L129"/>
+    <mergeCell ref="B127:L127"/>
+    <mergeCell ref="B135:Q135"/>
+    <mergeCell ref="E128:G128"/>
+    <mergeCell ref="B128:C129"/>
+    <mergeCell ref="D128:D129"/>
+    <mergeCell ref="H128:H129"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:C114"/>
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B117:E117"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="B109:C109"/>
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="B111:C111"/>
     <mergeCell ref="B95:E95"/>
+    <mergeCell ref="B103:G103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="B105:C105"/>
+    <mergeCell ref="B106:C106"/>
     <mergeCell ref="B62:G62"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="F24:F25"/>

</xml_diff>